<commit_message>
OFET fab table copy
added some of Ballantyne paper info
</commit_message>
<xml_diff>
--- a/OFET fab table copy.xlsx
+++ b/OFET fab table copy.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="125">
   <si>
     <t>Substrate Treatment</t>
   </si>
@@ -387,13 +387,22 @@
   </si>
   <si>
     <t>OFETConfig</t>
+  </si>
+  <si>
+    <t>1-2 microns</t>
+  </si>
+  <si>
+    <t>chlorobenzene</t>
+  </si>
+  <si>
+    <t>Ballantyne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +415,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -435,6 +445,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -910,17 +921,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -944,24 +946,21 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.138042730616912"/>
-          <c:y val="0.132738220892517"/>
-          <c:w val="0.806182651390125"/>
-          <c:h val="0.785755853998042"/>
+          <c:x val="0.13804273061691202"/>
+          <c:y val="0.13273822089251702"/>
+          <c:w val="0.80618265139012502"/>
+          <c:h val="0.78575585399804215"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -980,8 +979,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.181403196798207"/>
-                  <c:y val="0.091403073158444"/>
+                  <c:x val="0.18140319679820704"/>
+                  <c:y val="9.1403073158444009E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -994,13 +993,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>158.0</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.09</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.9</c:v>
@@ -1015,13 +1014,13 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>31.1</c:v>
@@ -1030,7 +1029,7 @@
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>31.1</c:v>
@@ -1039,25 +1038,25 @@
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>31.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.8</c:v>
+                  <c:v>33.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.6</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>13.4</c:v>
@@ -1078,61 +1077,61 @@
                   <c:v>31.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>40.3</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>13.8</c:v>
@@ -1147,58 +1146,58 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>76.0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>270.0</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>76.0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>270.0</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,204 +1215,203 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.86E-5</c:v>
+                  <c:v>4.8600000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>0.000551</c:v>
+                  <c:v>5.5099999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>0.00399</c:v>
+                  <c:v>3.9899999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0229</c:v>
+                  <c:v>2.29E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>0.0001921</c:v>
+                  <c:v>1.9210000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>0.000516</c:v>
+                  <c:v>5.1599999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>0.00067</c:v>
+                  <c:v>6.7000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>0.00783</c:v>
+                  <c:v>7.8300000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.014E-5</c:v>
+                  <c:v>7.0140000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>0.0009827</c:v>
+                  <c:v>9.8269999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0284</c:v>
+                  <c:v>2.8400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.43E-6</c:v>
+                  <c:v>5.4299999999999997E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>0.0003558</c:v>
+                  <c:v>3.5579999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>0.000735</c:v>
+                  <c:v>7.3499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>0.00748</c:v>
+                  <c:v>7.4799999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.61E-5</c:v>
+                  <c:v>1.6099999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>0.0005366</c:v>
+                  <c:v>5.3660000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>0.00419</c:v>
+                  <c:v>4.1900000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>0.00908</c:v>
+                  <c:v>9.0799999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.744E-6</c:v>
+                  <c:v>1.7439999999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>0.00785</c:v>
+                  <c:v>7.8499999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>0.00767</c:v>
+                  <c:v>7.6699999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>0.00423</c:v>
+                  <c:v>4.2300000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>0.00793</c:v>
+                  <c:v>7.9299999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0107</c:v>
+                  <c:v>1.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0165</c:v>
+                  <c:v>1.6500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0101</c:v>
+                  <c:v>1.01E-2</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>0.00892</c:v>
+                  <c:v>8.9200000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>0.0047</c:v>
+                  <c:v>4.7000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>0.00406</c:v>
+                  <c:v>4.0600000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>0.00214</c:v>
+                  <c:v>2.14E-3</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>0.00228</c:v>
+                  <c:v>2.2799999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>0.00279</c:v>
+                  <c:v>2.7899999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>0.000556</c:v>
+                  <c:v>5.5599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>0.000413</c:v>
+                  <c:v>4.1300000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>0.000426</c:v>
+                  <c:v>4.26E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>0.000254</c:v>
+                  <c:v>2.5399999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>0.000309</c:v>
+                  <c:v>3.0899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>0.000377</c:v>
+                  <c:v>3.77E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>0.0026</c:v>
+                  <c:v>2.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>0.0042</c:v>
+                  <c:v>4.1999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>0.0013</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>0.00047</c:v>
+                  <c:v>4.6999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.6E-5</c:v>
+                  <c:v>1.5999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3E-5</c:v>
+                  <c:v>4.3000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5E-7</c:v>
+                  <c:v>5.5000000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5E-6</c:v>
+                  <c:v>2.5000000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>0.0076</c:v>
+                  <c:v>7.6E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>0.00496</c:v>
+                  <c:v>4.96E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>0.00948</c:v>
+                  <c:v>9.4800000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.012</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>0.00529</c:v>
+                  <c:v>5.2900000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>0.00554</c:v>
+                  <c:v>5.5399999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>0.00299</c:v>
+                  <c:v>2.99E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>0.0081</c:v>
+                  <c:v>8.0999999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>0.0017</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>0.00149</c:v>
+                  <c:v>1.49E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0305</c:v>
+                  <c:v>3.0499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0631</c:v>
+                  <c:v>6.3100000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0775</c:v>
+                  <c:v>7.7499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0982</c:v>
+                  <c:v>9.8199999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1435</c:v>
+                  <c:v>0.14349999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1433,7 +1431,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.09</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9</c:v>
@@ -1448,7 +1446,7 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,21 +1458,20 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.000114</c:v>
+                  <c:v>1.1400000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000912</c:v>
+                  <c:v>9.1200000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00687</c:v>
+                  <c:v>6.8700000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.017</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1494,7 +1491,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.09</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9</c:v>
@@ -1509,13 +1506,13 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>31.1</c:v>
@@ -1524,25 +1521,25 @@
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>76.0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>270.0</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,76 +1551,67 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.46E-5</c:v>
+                  <c:v>1.4600000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000709</c:v>
+                  <c:v>7.0899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00414</c:v>
+                  <c:v>4.1399999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0364</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.08E-5</c:v>
+                  <c:v>5.0800000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00357</c:v>
+                  <c:v>3.5699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00994</c:v>
+                  <c:v>9.9399999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.0187</c:v>
+                  <c:v>1.8700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.0273</c:v>
+                  <c:v>2.7300000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.0539</c:v>
+                  <c:v>5.3900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.0612</c:v>
+                  <c:v>6.1199999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.0662</c:v>
+                  <c:v>6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.0652</c:v>
+                  <c:v>6.5199999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.0813</c:v>
+                  <c:v>8.1299999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2105032424"/>
-        <c:axId val="-2105026888"/>
+        <c:dLbls/>
+        <c:axId val="45946752"/>
+        <c:axId val="46384640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2105032424"/>
+        <c:axId val="45946752"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1645,27 +1633,23 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.117246985964707"/>
-              <c:y val="0.0801474166220286"/>
+              <c:x val="0.11724698596470701"/>
+              <c:y val="8.0147416622028581E-2"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105026888"/>
+        <c:crossAx val="46384640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105026888"/>
+        <c:axId val="46384640"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1684,13 +1668,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105032424"/>
+        <c:crossAx val="45946752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1701,21 +1682,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.690050452863255"/>
-          <c:y val="0.552787119863448"/>
-          <c:w val="0.145392413621326"/>
-          <c:h val="0.233839490629225"/>
+          <c:x val="0.69005045286325506"/>
+          <c:y val="0.55278711986344797"/>
+          <c:w val="0.14539241362132604"/>
+          <c:h val="0.23383949062922504"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1723,17 +1702,8 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1756,24 +1726,22 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0993423073927053"/>
-          <c:y val="0.132378576395413"/>
-          <c:w val="0.882890937222839"/>
-          <c:h val="0.82988191717607"/>
+          <c:x val="9.934230739270529E-2"/>
+          <c:y val="0.13237857639541298"/>
+          <c:w val="0.88289093722283907"/>
+          <c:h val="0.82988191717607018"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1787,10 +1755,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$BT$6</c:f>
+              <c:f>Sheet1!$D$6:$BS$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="69"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="1">
                   <c:v>1.31</c:v>
                 </c:pt>
@@ -1798,7 +1766,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.07</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.57</c:v>
@@ -1810,7 +1778,7 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.2</c:v>
@@ -1933,13 +1901,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>1.5</c:v>
@@ -1957,13 +1925,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1981,204 +1949,203 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.86E-5</c:v>
+                  <c:v>4.8600000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>0.000551</c:v>
+                  <c:v>5.5099999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>0.00399</c:v>
+                  <c:v>3.9899999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0229</c:v>
+                  <c:v>2.29E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>0.0001921</c:v>
+                  <c:v>1.9210000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>0.000516</c:v>
+                  <c:v>5.1599999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>0.00067</c:v>
+                  <c:v>6.7000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>0.00783</c:v>
+                  <c:v>7.8300000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.014E-5</c:v>
+                  <c:v>7.0140000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>0.0009827</c:v>
+                  <c:v>9.8269999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0284</c:v>
+                  <c:v>2.8400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.43E-6</c:v>
+                  <c:v>5.4299999999999997E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>0.0003558</c:v>
+                  <c:v>3.5579999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>0.000735</c:v>
+                  <c:v>7.3499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>0.00748</c:v>
+                  <c:v>7.4799999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.61E-5</c:v>
+                  <c:v>1.6099999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>0.0005366</c:v>
+                  <c:v>5.3660000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>0.00419</c:v>
+                  <c:v>4.1900000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>0.00908</c:v>
+                  <c:v>9.0799999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.744E-6</c:v>
+                  <c:v>1.7439999999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>0.00785</c:v>
+                  <c:v>7.8499999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>0.00767</c:v>
+                  <c:v>7.6699999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>0.00423</c:v>
+                  <c:v>4.2300000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>0.00793</c:v>
+                  <c:v>7.9299999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0107</c:v>
+                  <c:v>1.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0165</c:v>
+                  <c:v>1.6500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0101</c:v>
+                  <c:v>1.01E-2</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>0.00892</c:v>
+                  <c:v>8.9200000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>0.0047</c:v>
+                  <c:v>4.7000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>0.00406</c:v>
+                  <c:v>4.0600000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>0.00214</c:v>
+                  <c:v>2.14E-3</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>0.00228</c:v>
+                  <c:v>2.2799999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>0.00279</c:v>
+                  <c:v>2.7899999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>0.000556</c:v>
+                  <c:v>5.5599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>0.000413</c:v>
+                  <c:v>4.1300000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>0.000426</c:v>
+                  <c:v>4.26E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>0.000254</c:v>
+                  <c:v>2.5399999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>0.000309</c:v>
+                  <c:v>3.0899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>0.000377</c:v>
+                  <c:v>3.77E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>0.0026</c:v>
+                  <c:v>2.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>0.0042</c:v>
+                  <c:v>4.1999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>0.0013</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>0.00047</c:v>
+                  <c:v>4.6999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.6E-5</c:v>
+                  <c:v>1.5999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3E-5</c:v>
+                  <c:v>4.3000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5E-7</c:v>
+                  <c:v>5.5000000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5E-6</c:v>
+                  <c:v>2.5000000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>0.0076</c:v>
+                  <c:v>7.6E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>0.00496</c:v>
+                  <c:v>4.96E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>0.00948</c:v>
+                  <c:v>9.4800000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.012</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>0.00529</c:v>
+                  <c:v>5.2900000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>0.00554</c:v>
+                  <c:v>5.5399999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>0.00299</c:v>
+                  <c:v>2.99E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>0.0081</c:v>
+                  <c:v>8.0999999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>0.0017</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>0.00149</c:v>
+                  <c:v>1.49E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0305</c:v>
+                  <c:v>3.0499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0631</c:v>
+                  <c:v>6.3100000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0775</c:v>
+                  <c:v>7.7499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0982</c:v>
+                  <c:v>9.8199999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1435</c:v>
+                  <c:v>0.14349999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2204,7 +2171,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.07</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.57</c:v>
@@ -2225,21 +2192,20 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.000114</c:v>
+                  <c:v>1.1400000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000912</c:v>
+                  <c:v>9.1200000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00687</c:v>
+                  <c:v>6.8700000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.017</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2265,7 +2231,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.07</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.57</c:v>
@@ -2292,13 +2258,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2310,91 +2276,79 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.46E-5</c:v>
+                  <c:v>1.4600000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000709</c:v>
+                  <c:v>7.0899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00414</c:v>
+                  <c:v>4.1399999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0364</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.08E-5</c:v>
+                  <c:v>5.0800000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00357</c:v>
+                  <c:v>3.5699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00994</c:v>
+                  <c:v>9.9399999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.0187</c:v>
+                  <c:v>1.8700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.0273</c:v>
+                  <c:v>2.7300000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.0539</c:v>
+                  <c:v>5.3900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.0612</c:v>
+                  <c:v>6.1199999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.0662</c:v>
+                  <c:v>6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.0652</c:v>
+                  <c:v>6.5199999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.0813</c:v>
+                  <c:v>8.1299999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2104942280"/>
-        <c:axId val="-2104939288"/>
+        <c:dLbls/>
+        <c:axId val="46928256"/>
+        <c:axId val="46929792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104942280"/>
+        <c:axId val="46928256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104939288"/>
+        <c:crossAx val="46929792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104939288"/>
+        <c:axId val="46929792"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2417,13 +2371,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104942280"/>
+        <c:crossAx val="46928256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2434,21 +2386,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.210522396331926"/>
-          <c:y val="0.416321616485238"/>
-          <c:w val="0.0914527376443245"/>
-          <c:h val="0.174904439729482"/>
+          <c:x val="0.21052239633192604"/>
+          <c:y val="0.41632161648523802"/>
+          <c:w val="9.1452737644324489E-2"/>
+          <c:h val="0.17490443972948205"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2456,17 +2406,8 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2484,24 +2425,22 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0993423073927053"/>
-          <c:y val="0.132378576395413"/>
-          <c:w val="0.867528959813913"/>
-          <c:h val="0.82988191717607"/>
+          <c:x val="9.934230739270529E-2"/>
+          <c:y val="0.13237857639541298"/>
+          <c:w val="0.86752895981391298"/>
+          <c:h val="0.82988191717607018"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2526,205 +2465,205 @@
                   <c:v>10.839</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.58699999999997</c:v>
+                  <c:v>19.586999999999971</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19.58699999999997</c:v>
+                  <c:v>19.586999999999971</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.58699999999997</c:v>
+                  <c:v>19.586999999999971</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.34322349999995</c:v>
+                  <c:v>13.343223499999954</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.51525399999998</c:v>
+                  <c:v>13.515253999999976</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.87073600000002</c:v>
+                  <c:v>13.870736000000022</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14.24144599999997</c:v>
+                  <c:v>14.241445999999968</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>15.02854999999996</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>13.28439349999996</c:v>
+                  <c:v>13.284393499999956</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>13.39757399999998</c:v>
+                  <c:v>13.397573999999979</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>13.63529599999998</c:v>
+                  <c:v>13.635295999999977</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13.88816599999998</c:v>
+                  <c:v>13.888165999999975</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>14.43934999999997</c:v>
+                  <c:v>14.439349999999973</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.882999999999999</c:v>
+                  <c:v>6.8829999999999991</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.908210249999995</c:v>
+                  <c:v>6.9082102499999953</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.938981</c:v>
+                  <c:v>6.9389810000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.017203999999999</c:v>
+                  <c:v>7.0172039999999987</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.117668999999998</c:v>
+                  <c:v>7.1176689999999976</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.385324999999986</c:v>
+                  <c:v>7.3853249999999857</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>11.239</c:v>
+                  <c:v>11.239000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2742,204 +2681,203 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.86E-5</c:v>
+                  <c:v>4.8600000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>0.000551</c:v>
+                  <c:v>5.5099999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>0.00399</c:v>
+                  <c:v>3.9899999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0229</c:v>
+                  <c:v>2.29E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>0.0001921</c:v>
+                  <c:v>1.9210000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>0.000516</c:v>
+                  <c:v>5.1599999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>0.00067</c:v>
+                  <c:v>6.7000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>0.00783</c:v>
+                  <c:v>7.8300000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.014E-5</c:v>
+                  <c:v>7.0140000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>0.0009827</c:v>
+                  <c:v>9.8269999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0284</c:v>
+                  <c:v>2.8400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.43E-6</c:v>
+                  <c:v>5.4299999999999997E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>0.0003558</c:v>
+                  <c:v>3.5579999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>0.000735</c:v>
+                  <c:v>7.3499999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>0.00748</c:v>
+                  <c:v>7.4799999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.61E-5</c:v>
+                  <c:v>1.6099999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>0.0005366</c:v>
+                  <c:v>5.3660000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>0.00419</c:v>
+                  <c:v>4.1900000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>0.00908</c:v>
+                  <c:v>9.0799999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.744E-6</c:v>
+                  <c:v>1.7439999999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>0.00785</c:v>
+                  <c:v>7.8499999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>0.00767</c:v>
+                  <c:v>7.6699999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>0.00423</c:v>
+                  <c:v>4.2300000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>0.00793</c:v>
+                  <c:v>7.9299999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0107</c:v>
+                  <c:v>1.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0165</c:v>
+                  <c:v>1.6500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0101</c:v>
+                  <c:v>1.01E-2</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>0.00892</c:v>
+                  <c:v>8.9200000000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>0.0047</c:v>
+                  <c:v>4.7000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>0.00406</c:v>
+                  <c:v>4.0600000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>0.00214</c:v>
+                  <c:v>2.14E-3</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>0.00228</c:v>
+                  <c:v>2.2799999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>0.00279</c:v>
+                  <c:v>2.7899999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>0.000556</c:v>
+                  <c:v>5.5599999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>0.000413</c:v>
+                  <c:v>4.1300000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>0.000426</c:v>
+                  <c:v>4.26E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>0.000254</c:v>
+                  <c:v>2.5399999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>0.000309</c:v>
+                  <c:v>3.0899999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>0.000377</c:v>
+                  <c:v>3.77E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>0.0026</c:v>
+                  <c:v>2.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>0.0042</c:v>
+                  <c:v>4.1999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>0.0013</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>0.00047</c:v>
+                  <c:v>4.6999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.6E-5</c:v>
+                  <c:v>1.5999999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3E-5</c:v>
+                  <c:v>4.3000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5E-7</c:v>
+                  <c:v>5.5000000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5E-6</c:v>
+                  <c:v>2.5000000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>0.0076</c:v>
+                  <c:v>7.6E-3</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>0.00496</c:v>
+                  <c:v>4.96E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>0.00948</c:v>
+                  <c:v>9.4800000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.012</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>0.00529</c:v>
+                  <c:v>5.2900000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>0.00554</c:v>
+                  <c:v>5.5399999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>0.00299</c:v>
+                  <c:v>2.99E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>0.0081</c:v>
+                  <c:v>8.0999999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>0.0017</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>0.00149</c:v>
+                  <c:v>1.49E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0305</c:v>
+                  <c:v>3.0499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0631</c:v>
+                  <c:v>6.3100000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0775</c:v>
+                  <c:v>7.7499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0982</c:v>
+                  <c:v>9.8199999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1435</c:v>
+                  <c:v>0.14349999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2959,22 +2897,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2986,21 +2924,20 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.000114</c:v>
+                  <c:v>1.1400000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000912</c:v>
+                  <c:v>9.1200000000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00687</c:v>
+                  <c:v>6.8700000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.017</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3020,55 +2957,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.07347040000001</c:v>
+                  <c:v>17.073470400000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.17499999999998</c:v>
+                  <c:v>13.174999999999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3080,94 +3017,82 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.46E-5</c:v>
+                  <c:v>1.4600000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000709</c:v>
+                  <c:v>7.0899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00414</c:v>
+                  <c:v>4.1399999999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0364</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.08E-5</c:v>
+                  <c:v>5.0800000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00357</c:v>
+                  <c:v>3.5699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00615</c:v>
+                  <c:v>6.1500000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00994</c:v>
+                  <c:v>9.9399999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.0187</c:v>
+                  <c:v>1.8700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.0273</c:v>
+                  <c:v>2.7300000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.0539</c:v>
+                  <c:v>5.3900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.0612</c:v>
+                  <c:v>6.1199999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.0662</c:v>
+                  <c:v>6.6199999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.0652</c:v>
+                  <c:v>6.5199999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.0813</c:v>
+                  <c:v>8.1299999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2104902712"/>
-        <c:axId val="-2104899720"/>
+        <c:dLbls/>
+        <c:axId val="46978944"/>
+        <c:axId val="46980480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104902712"/>
+        <c:axId val="46978944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104899720"/>
+        <c:crossAx val="46980480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104899720"/>
+        <c:axId val="46980480"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:txPr>
             <a:bodyPr rot="-5400000" vert="horz"/>
             <a:lstStyle/>
@@ -3180,10 +3105,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2104902712"/>
+        <c:crossAx val="46978944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3194,21 +3117,19 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.84885986899397"/>
-          <c:y val="0.323424369891966"/>
-          <c:w val="0.0808354682410482"/>
-          <c:h val="0.174904439729482"/>
+          <c:x val="0.84885986899397015"/>
+          <c:y val="0.32342436989196616"/>
+          <c:w val="8.0835468241048203E-2"/>
+          <c:h val="0.17490443972948205"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3599,21 +3520,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BS134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:BY134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="4940" topLeftCell="BJ1" activePane="topRight"/>
-      <selection activeCell="A12" sqref="A12:XFD12"/>
-      <selection pane="topRight" activeCell="BT3" sqref="BT3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="3210" topLeftCell="BD1" activePane="topRight"/>
+      <selection activeCell="B12" sqref="B12"/>
+      <selection pane="topRight" activeCell="BT4" sqref="BT4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:71">
+    <row r="2" spans="1:77">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3824,8 +3745,26 @@
       <c r="BS2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:71">
+      <c r="BT2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BY2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:77">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -4036,8 +3975,26 @@
       <c r="BS3">
         <v>2006</v>
       </c>
-    </row>
-    <row r="4" spans="1:71">
+      <c r="BT3">
+        <v>2008</v>
+      </c>
+      <c r="BU3">
+        <v>2008</v>
+      </c>
+      <c r="BV3">
+        <v>2008</v>
+      </c>
+      <c r="BW3">
+        <v>2008</v>
+      </c>
+      <c r="BX3">
+        <v>2008</v>
+      </c>
+      <c r="BY3">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -4246,7 +4203,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:71" s="4" customFormat="1">
+    <row r="5" spans="1:77" s="4" customFormat="1">
       <c r="B5" s="4" t="s">
         <v>96</v>
       </c>
@@ -4457,8 +4414,26 @@
       <c r="BS5" s="4">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:71" s="4" customFormat="1">
+      <c r="BT5" s="4">
+        <v>13</v>
+      </c>
+      <c r="BU5" s="4">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="BV5" s="4">
+        <v>34.4</v>
+      </c>
+      <c r="BW5" s="4">
+        <v>55.6</v>
+      </c>
+      <c r="BX5" s="4">
+        <v>85</v>
+      </c>
+      <c r="BY5" s="4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:77" s="4" customFormat="1">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -4636,8 +4611,26 @@
       <c r="BS6" s="4">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:71" s="4" customFormat="1">
+      <c r="BT6" s="4">
+        <v>2</v>
+      </c>
+      <c r="BU6" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="BV6" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="BW6" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="BX6" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="BY6" s="4">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:77" s="4" customFormat="1">
       <c r="B7" s="4" t="s">
         <v>97</v>
       </c>
@@ -4842,8 +4835,26 @@
       <c r="BS7" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:71" s="5" customFormat="1">
+      <c r="BT7" s="4">
+        <v>97</v>
+      </c>
+      <c r="BU7" s="4">
+        <v>97</v>
+      </c>
+      <c r="BV7" s="4">
+        <v>97</v>
+      </c>
+      <c r="BW7" s="4">
+        <v>97</v>
+      </c>
+      <c r="BX7" s="4">
+        <v>97</v>
+      </c>
+      <c r="BY7" s="4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:77" s="5" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>114</v>
       </c>
@@ -5031,7 +5042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:71" s="5" customFormat="1">
+    <row r="9" spans="1:77" s="5" customFormat="1">
       <c r="B9" s="5" t="s">
         <v>115</v>
       </c>
@@ -5242,8 +5253,26 @@
       <c r="BS9" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:71" s="5" customFormat="1">
+      <c r="BT9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BU9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BV9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BW9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BX9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BY9" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:77" s="5" customFormat="1">
       <c r="B10" s="5" t="s">
         <v>116</v>
       </c>
@@ -5293,7 +5322,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:71" s="5" customFormat="1">
+    <row r="11" spans="1:77" s="5" customFormat="1">
       <c r="B11" s="5" t="s">
         <v>117</v>
       </c>
@@ -5343,7 +5372,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:71" s="5" customFormat="1">
+    <row r="12" spans="1:77" s="5" customFormat="1">
       <c r="B12" s="5" t="s">
         <v>87</v>
       </c>
@@ -5624,7 +5653,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="13" spans="1:71" s="14" customFormat="1">
+    <row r="13" spans="1:77" s="14" customFormat="1">
       <c r="B13" s="14" t="s">
         <v>98</v>
       </c>
@@ -5905,7 +5934,7 @@
         <v>11.239000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:71" s="5" customFormat="1">
+    <row r="14" spans="1:77" s="5" customFormat="1">
       <c r="B14" s="5" t="s">
         <v>99</v>
       </c>
@@ -5958,7 +5987,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:71" s="5" customFormat="1">
+    <row r="15" spans="1:77" s="5" customFormat="1">
       <c r="B15" s="5" t="s">
         <v>100</v>
       </c>
@@ -6089,7 +6118,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:71" s="5" customFormat="1">
+    <row r="16" spans="1:77" s="5" customFormat="1">
       <c r="B16" s="5" t="s">
         <v>101</v>
       </c>
@@ -6220,7 +6249,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:71" s="6" customFormat="1">
+    <row r="17" spans="2:77" s="6" customFormat="1">
       <c r="B17" s="6" t="s">
         <v>102</v>
       </c>
@@ -6381,7 +6410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:71" s="7" customFormat="1">
+    <row r="18" spans="2:77" s="7" customFormat="1">
       <c r="B18" s="7" t="s">
         <v>103</v>
       </c>
@@ -6592,8 +6621,26 @@
       <c r="BS18" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:71" s="7" customFormat="1">
+      <c r="BT18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="BU18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="BV18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="BW18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="BX18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="BY18" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:77" s="7" customFormat="1">
       <c r="B19" s="7" t="s">
         <v>104</v>
       </c>
@@ -6775,7 +6822,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="2:71" s="7" customFormat="1">
+    <row r="20" spans="2:77" s="7" customFormat="1">
       <c r="B20" s="7" t="s">
         <v>105</v>
       </c>
@@ -6849,7 +6896,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:71" s="7" customFormat="1">
+    <row r="21" spans="2:77" s="7" customFormat="1">
       <c r="B21" s="7" t="s">
         <v>106</v>
       </c>
@@ -7003,8 +7050,26 @@
       <c r="BS21" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="2:71">
+      <c r="BT21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BU21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BV21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BW21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BX21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY21" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="2:77">
       <c r="B22" t="s">
         <v>107</v>
       </c>
@@ -7077,8 +7142,26 @@
       <c r="BS22" s="12">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="2:71">
+      <c r="BT22" s="12">
+        <v>140</v>
+      </c>
+      <c r="BU22" s="12">
+        <v>140</v>
+      </c>
+      <c r="BV22" s="12">
+        <v>140</v>
+      </c>
+      <c r="BW22" s="12">
+        <v>150</v>
+      </c>
+      <c r="BX22" s="12">
+        <v>150</v>
+      </c>
+      <c r="BY22" s="12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:77">
       <c r="B23" t="s">
         <v>108</v>
       </c>
@@ -7155,8 +7238,26 @@
       <c r="BS23" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:71">
+      <c r="BT23" s="12">
+        <v>2</v>
+      </c>
+      <c r="BU23" s="12">
+        <v>2</v>
+      </c>
+      <c r="BV23" s="12">
+        <v>2</v>
+      </c>
+      <c r="BW23" s="12">
+        <v>2</v>
+      </c>
+      <c r="BX23" s="12">
+        <v>2</v>
+      </c>
+      <c r="BY23" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:77">
       <c r="B24" t="s">
         <v>109</v>
       </c>
@@ -7183,7 +7284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:71" s="8" customFormat="1">
+    <row r="25" spans="2:77" s="8" customFormat="1">
       <c r="B25" s="8" t="s">
         <v>110</v>
       </c>
@@ -7394,8 +7495,26 @@
       <c r="BS25" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:71" s="8" customFormat="1">
+      <c r="BT25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BU25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BV25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BW25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BX25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BY25" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:77" s="8" customFormat="1">
       <c r="B26" s="8" t="s">
         <v>120</v>
       </c>
@@ -7607,7 +7726,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:71" s="8" customFormat="1">
+    <row r="27" spans="2:77" s="8" customFormat="1">
       <c r="B27" s="8" t="s">
         <v>121</v>
       </c>
@@ -7813,7 +7932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:71" s="8" customFormat="1">
+    <row r="28" spans="2:77" s="8" customFormat="1">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
@@ -7866,7 +7985,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="2:71" s="8" customFormat="1">
+    <row r="29" spans="2:77" s="8" customFormat="1">
       <c r="B29" s="8" t="s">
         <v>112</v>
       </c>
@@ -7919,7 +8038,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:71" s="8" customFormat="1">
+    <row r="30" spans="2:77" s="8" customFormat="1">
       <c r="B30" s="8" t="s">
         <v>113</v>
       </c>
@@ -8124,8 +8243,26 @@
       <c r="BS30" s="8">
         <v>0.14349999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="2:71">
+      <c r="BT30" s="9">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="BU30" s="9">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="BV30" s="9">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="BW30" s="9">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="BX30" s="9">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="BY30" s="9">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:77">
       <c r="C31">
         <v>1</v>
       </c>
@@ -8401,8 +8538,32 @@
         <f t="shared" si="5"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="2:71" s="2" customFormat="1" ht="78" customHeight="1">
+      <c r="BT31">
+        <f t="shared" ref="BT31" si="6">BS31+1</f>
+        <v>70</v>
+      </c>
+      <c r="BU31">
+        <f t="shared" ref="BU31" si="7">BT31+1</f>
+        <v>71</v>
+      </c>
+      <c r="BV31">
+        <f t="shared" ref="BV31" si="8">BU31+1</f>
+        <v>72</v>
+      </c>
+      <c r="BW31">
+        <f t="shared" ref="BW31" si="9">BV31+1</f>
+        <v>73</v>
+      </c>
+      <c r="BX31">
+        <f t="shared" ref="BX31" si="10">BW31+1</f>
+        <v>74</v>
+      </c>
+      <c r="BY31">
+        <f t="shared" ref="BY31" si="11">BX31+1</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:77" s="2" customFormat="1" ht="78" customHeight="1">
       <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
@@ -8628,23 +8789,23 @@
         <v>334</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" ref="D44:E44" si="6">IF(ISBLANK(D42),LOOKUP(D41,$A$100:$A$108,$F$100:$F$108),D43*LOOKUP(D41,$A$100:$A$108,$F$100:$F$108)+(1-D43)*LOOKUP(D42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="D44:E44" si="12">IF(ISBLANK(D42),LOOKUP(D41,$A$100:$A$108,$F$100:$F$108),D43*LOOKUP(D41,$A$100:$A$108,$F$100:$F$108)+(1-D43)*LOOKUP(D42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>334</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" ref="F44:G44" si="7">IF(ISBLANK(F42),LOOKUP(F41,$A$100:$A$108,$F$100:$F$108),F43*LOOKUP(F41,$A$100:$A$108,$F$100:$F$108)+(1-F43)*LOOKUP(F42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="F44:G44" si="13">IF(ISBLANK(F42),LOOKUP(F41,$A$100:$A$108,$F$100:$F$108),F43*LOOKUP(F41,$A$100:$A$108,$F$100:$F$108)+(1-F43)*LOOKUP(F42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="G44" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>334</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" ref="H44" si="8">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="H44" si="14">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
     </row>
@@ -8657,23 +8818,23 @@
         <v>13.174999999999979</v>
       </c>
       <c r="D45" s="14">
-        <f t="shared" ref="D45:H45" si="9">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D45:H45" si="15">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>13.174999999999979</v>
       </c>
       <c r="E45" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>13.174999999999979</v>
       </c>
       <c r="F45" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>13.174999999999979</v>
       </c>
       <c r="G45" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>13.174999999999979</v>
       </c>
       <c r="H45" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>13.174999999999979</v>
       </c>
     </row>
@@ -8905,19 +9066,19 @@
         <v>71</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:H62" si="10">D62+1</f>
+        <f t="shared" ref="E62:H62" si="16">D62+1</f>
         <v>72</v>
       </c>
       <c r="F62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>73</v>
       </c>
       <c r="G62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>74</v>
       </c>
       <c r="H62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>75</v>
       </c>
     </row>
@@ -9423,67 +9584,67 @@
         <v>334.88</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" ref="D75:E75" si="11">IF(ISBLANK(D73),LOOKUP(D72,$A$100:$A$108,$F$100:$F$108),D74*LOOKUP(D72,$A$100:$A$108,$F$100:$F$108)+(1-D74)*LOOKUP(D73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="D75:E75" si="17">IF(ISBLANK(D73),LOOKUP(D72,$A$100:$A$108,$F$100:$F$108),D74*LOOKUP(D72,$A$100:$A$108,$F$100:$F$108)+(1-D74)*LOOKUP(D73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>334.88</v>
       </c>
       <c r="F75" s="5">
-        <f t="shared" ref="F75:G75" si="12">IF(ISBLANK(F73),LOOKUP(F72,$A$100:$A$108,$F$100:$F$108),F74*LOOKUP(F72,$A$100:$A$108,$F$100:$F$108)+(1-F74)*LOOKUP(F73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="F75:G75" si="18">IF(ISBLANK(F73),LOOKUP(F72,$A$100:$A$108,$F$100:$F$108),F74*LOOKUP(F72,$A$100:$A$108,$F$100:$F$108)+(1-F74)*LOOKUP(F73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="G75" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>334.88</v>
       </c>
       <c r="H75" s="5">
-        <f t="shared" ref="H75:I75" si="13">IF(ISBLANK(H73),LOOKUP(H72,$A$100:$A$108,$F$100:$F$108),H74*LOOKUP(H72,$A$100:$A$108,$F$100:$F$108)+(1-H74)*LOOKUP(H73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="H75:I75" si="19">IF(ISBLANK(H73),LOOKUP(H72,$A$100:$A$108,$F$100:$F$108),H74*LOOKUP(H72,$A$100:$A$108,$F$100:$F$108)+(1-H74)*LOOKUP(H73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="I75" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>334</v>
       </c>
       <c r="J75" s="5">
-        <f t="shared" ref="J75:K75" si="14">IF(ISBLANK(J73),LOOKUP(J72,$A$100:$A$108,$F$100:$F$108),J74*LOOKUP(J72,$A$100:$A$108,$F$100:$F$108)+(1-J74)*LOOKUP(J73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="J75:K75" si="20">IF(ISBLANK(J73),LOOKUP(J72,$A$100:$A$108,$F$100:$F$108),J74*LOOKUP(J72,$A$100:$A$108,$F$100:$F$108)+(1-J74)*LOOKUP(J73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="K75" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>334</v>
       </c>
       <c r="L75" s="5">
-        <f t="shared" ref="L75:M75" si="15">IF(ISBLANK(L73),LOOKUP(L72,$A$100:$A$108,$F$100:$F$108),L74*LOOKUP(L72,$A$100:$A$108,$F$100:$F$108)+(1-L74)*LOOKUP(L73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="L75:M75" si="21">IF(ISBLANK(L73),LOOKUP(L72,$A$100:$A$108,$F$100:$F$108),L74*LOOKUP(L72,$A$100:$A$108,$F$100:$F$108)+(1-L74)*LOOKUP(L73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="M75" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>334</v>
       </c>
       <c r="N75" s="5">
-        <f t="shared" ref="N75:O75" si="16">IF(ISBLANK(N73),LOOKUP(N72,$A$100:$A$108,$F$100:$F$108),N74*LOOKUP(N72,$A$100:$A$108,$F$100:$F$108)+(1-N74)*LOOKUP(N73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="N75:O75" si="22">IF(ISBLANK(N73),LOOKUP(N72,$A$100:$A$108,$F$100:$F$108),N74*LOOKUP(N72,$A$100:$A$108,$F$100:$F$108)+(1-N74)*LOOKUP(N73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="O75" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>334</v>
       </c>
       <c r="P75" s="5">
-        <f t="shared" ref="P75:Q75" si="17">IF(ISBLANK(P73),LOOKUP(P72,$A$100:$A$108,$F$100:$F$108),P74*LOOKUP(P72,$A$100:$A$108,$F$100:$F$108)+(1-P74)*LOOKUP(P73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="P75:Q75" si="23">IF(ISBLANK(P73),LOOKUP(P72,$A$100:$A$108,$F$100:$F$108),P74*LOOKUP(P72,$A$100:$A$108,$F$100:$F$108)+(1-P74)*LOOKUP(P73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="Q75" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>334</v>
       </c>
       <c r="R75" s="5">
-        <f t="shared" ref="R75:S75" si="18">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="R75:S75" si="24">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="S75" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>334</v>
       </c>
     </row>
@@ -9496,67 +9657,67 @@
         <v>17.073470400000005</v>
       </c>
       <c r="D76" s="14">
-        <f t="shared" ref="D76:S76" si="19">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D76:S76" si="25">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>17.073470400000005</v>
       </c>
       <c r="E76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>17.073470400000005</v>
       </c>
       <c r="F76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>17.073470400000005</v>
       </c>
       <c r="G76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>17.073470400000005</v>
       </c>
       <c r="H76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>17.073470400000005</v>
       </c>
       <c r="I76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="K76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="L76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="M76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="N76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="O76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="P76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="Q76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="R76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
       <c r="S76" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>13.174999999999979</v>
       </c>
     </row>
@@ -10226,63 +10387,63 @@
         <v>77</v>
       </c>
       <c r="E93">
-        <f t="shared" ref="E93:S93" si="20">D93+1</f>
+        <f t="shared" ref="E93:S93" si="26">D93+1</f>
         <v>78</v>
       </c>
       <c r="F93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>79</v>
       </c>
       <c r="G93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>80</v>
       </c>
       <c r="H93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>81</v>
       </c>
       <c r="I93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>82</v>
       </c>
       <c r="J93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>83</v>
       </c>
       <c r="K93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="L93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>85</v>
       </c>
       <c r="M93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>86</v>
       </c>
       <c r="N93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>87</v>
       </c>
       <c r="O93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>88</v>
       </c>
       <c r="P93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>89</v>
       </c>
       <c r="Q93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>90</v>
       </c>
       <c r="R93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>91</v>
       </c>
       <c r="S93">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>92</v>
       </c>
     </row>
@@ -10632,12 +10793,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -10649,12 +10810,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Removed Ballantyne, Figure out Surin stuff
Will have to change the formula for keeping counts of devices
</commit_message>
<xml_diff>
--- a/OFET fab table copy.xlsx
+++ b/OFET fab table copy.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="132">
   <si>
     <t>Substrate Treatment</t>
   </si>
@@ -389,15 +389,6 @@
     <t>OFETConfig</t>
   </si>
   <si>
-    <t>1-2 microns</t>
-  </si>
-  <si>
-    <t>chlorobenzene</t>
-  </si>
-  <si>
-    <t>Ballantyne</t>
-  </si>
-  <si>
     <t>Surin</t>
   </si>
   <si>
@@ -411,13 +402,28 @@
   </si>
   <si>
     <t>N4</t>
+  </si>
+  <si>
+    <t>accumulation</t>
+  </si>
+  <si>
+    <t>10 µm</t>
+  </si>
+  <si>
+    <t>61 s</t>
+  </si>
+  <si>
+    <t>11 µm</t>
+  </si>
+  <si>
+    <t>10.1063/1.2222065</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,8 +523,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -731,7 +739,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -827,6 +835,7 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -922,6 +931,7 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -936,8 +946,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -961,21 +980,24 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13804273061691202"/>
-          <c:y val="0.13273822089251702"/>
-          <c:w val="0.80618265139012502"/>
-          <c:h val="0.78575585399804215"/>
+          <c:x val="0.138042730616912"/>
+          <c:y val="0.132738220892517"/>
+          <c:w val="0.806182651390125"/>
+          <c:h val="0.785755853998042"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -994,8 +1016,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.18140319679820704"/>
-                  <c:y val="9.1403073158444009E-2"/>
+                  <c:x val="0.181403196798207"/>
+                  <c:y val="0.091403073158444"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1008,13 +1030,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="69"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>158</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.9</c:v>
@@ -1029,13 +1051,13 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>31.1</c:v>
@@ -1044,7 +1066,7 @@
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>31.1</c:v>
@@ -1053,25 +1075,25 @@
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>31.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.799999999999997</c:v>
+                  <c:v>33.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4.6</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>13.4</c:v>
@@ -1092,61 +1114,61 @@
                   <c:v>31.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>40.3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>13.8</c:v>
@@ -1161,58 +1183,58 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>76</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>76</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1230,203 +1252,204 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.8600000000000002E-5</c:v>
+                  <c:v>4.86E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.5099999999999995E-4</c:v>
+                  <c:v>0.000551</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>3.9899999999999996E-3</c:v>
+                  <c:v>0.00399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.29E-2</c:v>
+                  <c:v>0.0229</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1.9210000000000001E-4</c:v>
+                  <c:v>0.0001921</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>5.1599999999999997E-4</c:v>
+                  <c:v>0.000516</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>6.7000000000000002E-4</c:v>
+                  <c:v>0.00067</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>7.8300000000000002E-3</c:v>
+                  <c:v>0.00783</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.0140000000000003E-5</c:v>
+                  <c:v>7.014E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>9.8269999999999998E-4</c:v>
+                  <c:v>0.0009827</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.8400000000000002E-2</c:v>
+                  <c:v>0.0284</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.4299999999999997E-6</c:v>
+                  <c:v>5.43E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>3.5579999999999997E-4</c:v>
+                  <c:v>0.0003558</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>7.3499999999999998E-4</c:v>
+                  <c:v>0.000735</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>7.4799999999999997E-3</c:v>
+                  <c:v>0.00748</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.6099999999999998E-5</c:v>
+                  <c:v>1.61E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>5.3660000000000003E-4</c:v>
+                  <c:v>0.0005366</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.1900000000000001E-3</c:v>
+                  <c:v>0.00419</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>9.0799999999999995E-3</c:v>
+                  <c:v>0.00908</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.7439999999999999E-6</c:v>
+                  <c:v>1.744E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.8499999999999993E-3</c:v>
+                  <c:v>0.00785</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>7.6699999999999997E-3</c:v>
+                  <c:v>0.00767</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>4.2300000000000003E-3</c:v>
+                  <c:v>0.00423</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>7.9299999999999995E-3</c:v>
+                  <c:v>0.00793</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0699999999999999E-2</c:v>
+                  <c:v>0.0107</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>0.0165</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.01E-2</c:v>
+                  <c:v>0.0101</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>8.9200000000000008E-3</c:v>
+                  <c:v>0.00892</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>4.7000000000000002E-3</c:v>
+                  <c:v>0.0047</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>4.0600000000000002E-3</c:v>
+                  <c:v>0.00406</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>2.14E-3</c:v>
+                  <c:v>0.00214</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>2.2799999999999999E-3</c:v>
+                  <c:v>0.00228</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>2.7899999999999999E-3</c:v>
+                  <c:v>0.00279</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>5.5599999999999996E-4</c:v>
+                  <c:v>0.000556</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.1300000000000001E-4</c:v>
+                  <c:v>0.000413</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.26E-4</c:v>
+                  <c:v>0.000426</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>2.5399999999999999E-4</c:v>
+                  <c:v>0.000254</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.0899999999999998E-4</c:v>
+                  <c:v>0.000309</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.77E-4</c:v>
+                  <c:v>0.000377</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>2.5999999999999999E-3</c:v>
+                  <c:v>0.0026</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.1999999999999997E-3</c:v>
+                  <c:v>0.0042</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>0.0013</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.6999999999999999E-4</c:v>
+                  <c:v>0.00047</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.5999999999999999E-5</c:v>
+                  <c:v>1.6E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3000000000000002E-5</c:v>
+                  <c:v>4.3E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5000000000000003E-7</c:v>
+                  <c:v>5.5E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5000000000000002E-6</c:v>
+                  <c:v>2.5E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.6E-3</c:v>
+                  <c:v>0.0076</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.96E-3</c:v>
+                  <c:v>0.00496</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>9.4800000000000006E-3</c:v>
+                  <c:v>0.00948</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>0.012</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>5.2900000000000004E-3</c:v>
+                  <c:v>0.00529</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>5.5399999999999998E-3</c:v>
+                  <c:v>0.00554</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>2.99E-3</c:v>
+                  <c:v>0.00299</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>8.0999999999999996E-3</c:v>
+                  <c:v>0.0081</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>0.0017</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.49E-3</c:v>
+                  <c:v>0.00149</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.0499999999999999E-2</c:v>
+                  <c:v>0.0305</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.3100000000000003E-2</c:v>
+                  <c:v>0.0631</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.7499999999999999E-2</c:v>
+                  <c:v>0.0775</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>9.8199999999999996E-2</c:v>
+                  <c:v>0.0982</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.14349999999999999</c:v>
+                  <c:v>0.1435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1446,7 +1469,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9</c:v>
@@ -1461,7 +1484,7 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,20 +1496,21 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1.1400000000000001E-4</c:v>
+                  <c:v>0.000114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1200000000000005E-4</c:v>
+                  <c:v>0.000912</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8700000000000002E-3</c:v>
+                  <c:v>0.00687</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>0.017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1506,7 +1530,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>1.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.9</c:v>
@@ -1521,13 +1545,13 @@
                   <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>31.1</c:v>
@@ -1536,25 +1560,25 @@
                   <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>52.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>76</c:v>
+                  <c:v>76.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>270</c:v>
+                  <c:v>270.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,67 +1590,76 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.4600000000000001E-5</c:v>
+                  <c:v>1.46E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0899999999999999E-4</c:v>
+                  <c:v>0.000709</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1399999999999996E-3</c:v>
+                  <c:v>0.00414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6400000000000002E-2</c:v>
+                  <c:v>0.0364</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0800000000000002E-5</c:v>
+                  <c:v>5.08E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5699999999999998E-3</c:v>
+                  <c:v>0.00357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9399999999999992E-3</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.8700000000000001E-2</c:v>
+                  <c:v>0.0187</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.7300000000000001E-2</c:v>
+                  <c:v>0.0273</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.3900000000000003E-2</c:v>
+                  <c:v>0.0539</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>6.1199999999999997E-2</c:v>
+                  <c:v>0.0612</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>0.0662</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>6.5199999999999994E-2</c:v>
+                  <c:v>0.0652</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>8.1299999999999997E-2</c:v>
+                  <c:v>0.0813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="45946752"/>
-        <c:axId val="46384640"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2129949896"/>
+        <c:axId val="2129955416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45946752"/>
+        <c:axId val="2129949896"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1648,23 +1681,27 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.11724698596470701"/>
-              <c:y val="8.0147416622028581E-2"/>
+              <c:x val="0.117246985964707"/>
+              <c:y val="0.0801474166220286"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46384640"/>
+        <c:crossAx val="2129955416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46384640"/>
+        <c:axId val="2129955416"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1683,10 +1720,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45946752"/>
+        <c:crossAx val="2129949896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1697,19 +1737,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.69005045286325506"/>
-          <c:y val="0.55278711986344797"/>
-          <c:w val="0.14539241362132604"/>
-          <c:h val="0.23383949062922504"/>
+          <c:x val="0.690050452863255"/>
+          <c:y val="0.552787119863448"/>
+          <c:w val="0.145392413621326"/>
+          <c:h val="0.233839490629225"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1717,8 +1759,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1742,21 +1793,24 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.934230739270529E-2"/>
-          <c:y val="0.13237857639541298"/>
-          <c:w val="0.88289093722283907"/>
-          <c:h val="0.82988191717607018"/>
+          <c:x val="0.0993423073927053"/>
+          <c:y val="0.132378576395413"/>
+          <c:w val="0.882890937222839"/>
+          <c:h val="0.82988191717607"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1781,7 +1835,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0699999999999998</c:v>
+                  <c:v>2.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.57</c:v>
@@ -1793,7 +1847,7 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.2</c:v>
@@ -1916,13 +1970,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>1.5</c:v>
@@ -1940,13 +1994,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1964,203 +2018,204 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.8600000000000002E-5</c:v>
+                  <c:v>4.86E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.5099999999999995E-4</c:v>
+                  <c:v>0.000551</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>3.9899999999999996E-3</c:v>
+                  <c:v>0.00399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.29E-2</c:v>
+                  <c:v>0.0229</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1.9210000000000001E-4</c:v>
+                  <c:v>0.0001921</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>5.1599999999999997E-4</c:v>
+                  <c:v>0.000516</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>6.7000000000000002E-4</c:v>
+                  <c:v>0.00067</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>7.8300000000000002E-3</c:v>
+                  <c:v>0.00783</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.0140000000000003E-5</c:v>
+                  <c:v>7.014E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>9.8269999999999998E-4</c:v>
+                  <c:v>0.0009827</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.8400000000000002E-2</c:v>
+                  <c:v>0.0284</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.4299999999999997E-6</c:v>
+                  <c:v>5.43E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>3.5579999999999997E-4</c:v>
+                  <c:v>0.0003558</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>7.3499999999999998E-4</c:v>
+                  <c:v>0.000735</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>7.4799999999999997E-3</c:v>
+                  <c:v>0.00748</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.6099999999999998E-5</c:v>
+                  <c:v>1.61E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>5.3660000000000003E-4</c:v>
+                  <c:v>0.0005366</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.1900000000000001E-3</c:v>
+                  <c:v>0.00419</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>9.0799999999999995E-3</c:v>
+                  <c:v>0.00908</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.7439999999999999E-6</c:v>
+                  <c:v>1.744E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.8499999999999993E-3</c:v>
+                  <c:v>0.00785</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>7.6699999999999997E-3</c:v>
+                  <c:v>0.00767</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>4.2300000000000003E-3</c:v>
+                  <c:v>0.00423</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>7.9299999999999995E-3</c:v>
+                  <c:v>0.00793</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0699999999999999E-2</c:v>
+                  <c:v>0.0107</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>0.0165</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.01E-2</c:v>
+                  <c:v>0.0101</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>8.9200000000000008E-3</c:v>
+                  <c:v>0.00892</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>4.7000000000000002E-3</c:v>
+                  <c:v>0.0047</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>4.0600000000000002E-3</c:v>
+                  <c:v>0.00406</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>2.14E-3</c:v>
+                  <c:v>0.00214</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>2.2799999999999999E-3</c:v>
+                  <c:v>0.00228</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>2.7899999999999999E-3</c:v>
+                  <c:v>0.00279</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>5.5599999999999996E-4</c:v>
+                  <c:v>0.000556</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.1300000000000001E-4</c:v>
+                  <c:v>0.000413</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.26E-4</c:v>
+                  <c:v>0.000426</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>2.5399999999999999E-4</c:v>
+                  <c:v>0.000254</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.0899999999999998E-4</c:v>
+                  <c:v>0.000309</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.77E-4</c:v>
+                  <c:v>0.000377</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>2.5999999999999999E-3</c:v>
+                  <c:v>0.0026</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.1999999999999997E-3</c:v>
+                  <c:v>0.0042</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>0.0013</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.6999999999999999E-4</c:v>
+                  <c:v>0.00047</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.5999999999999999E-5</c:v>
+                  <c:v>1.6E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3000000000000002E-5</c:v>
+                  <c:v>4.3E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5000000000000003E-7</c:v>
+                  <c:v>5.5E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5000000000000002E-6</c:v>
+                  <c:v>2.5E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.6E-3</c:v>
+                  <c:v>0.0076</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.96E-3</c:v>
+                  <c:v>0.00496</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>9.4800000000000006E-3</c:v>
+                  <c:v>0.00948</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>0.012</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>5.2900000000000004E-3</c:v>
+                  <c:v>0.00529</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>5.5399999999999998E-3</c:v>
+                  <c:v>0.00554</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>2.99E-3</c:v>
+                  <c:v>0.00299</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>8.0999999999999996E-3</c:v>
+                  <c:v>0.0081</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>0.0017</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.49E-3</c:v>
+                  <c:v>0.00149</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.0499999999999999E-2</c:v>
+                  <c:v>0.0305</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.3100000000000003E-2</c:v>
+                  <c:v>0.0631</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.7499999999999999E-2</c:v>
+                  <c:v>0.0775</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>9.8199999999999996E-2</c:v>
+                  <c:v>0.0982</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.14349999999999999</c:v>
+                  <c:v>0.1435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2186,7 +2241,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0699999999999998</c:v>
+                  <c:v>2.07</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.57</c:v>
@@ -2207,20 +2262,21 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1.1400000000000001E-4</c:v>
+                  <c:v>0.000114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1200000000000005E-4</c:v>
+                  <c:v>0.000912</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8700000000000002E-3</c:v>
+                  <c:v>0.00687</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>0.017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2246,7 +2302,7 @@
                   <c:v>1.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0699999999999998</c:v>
+                  <c:v>2.07</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.57</c:v>
@@ -2273,13 +2329,13 @@
                   <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,79 +2347,91 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.4600000000000001E-5</c:v>
+                  <c:v>1.46E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0899999999999999E-4</c:v>
+                  <c:v>0.000709</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1399999999999996E-3</c:v>
+                  <c:v>0.00414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6400000000000002E-2</c:v>
+                  <c:v>0.0364</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0800000000000002E-5</c:v>
+                  <c:v>5.08E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5699999999999998E-3</c:v>
+                  <c:v>0.00357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9399999999999992E-3</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.8700000000000001E-2</c:v>
+                  <c:v>0.0187</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.7300000000000001E-2</c:v>
+                  <c:v>0.0273</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.3900000000000003E-2</c:v>
+                  <c:v>0.0539</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>6.1199999999999997E-2</c:v>
+                  <c:v>0.0612</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>0.0662</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>6.5199999999999994E-2</c:v>
+                  <c:v>0.0652</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>8.1299999999999997E-2</c:v>
+                  <c:v>0.0813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="46928256"/>
-        <c:axId val="46929792"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2130058168"/>
+        <c:axId val="2130061240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46928256"/>
+        <c:axId val="2130058168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46929792"/>
+        <c:crossAx val="2130061240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46929792"/>
+        <c:axId val="2130061240"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2387,10 +2455,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46928256"/>
+        <c:crossAx val="2130058168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2401,19 +2472,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.21052239633192604"/>
-          <c:y val="0.41632161648523802"/>
-          <c:w val="9.1452737644324489E-2"/>
-          <c:h val="0.17490443972948205"/>
+          <c:x val="0.210522396331926"/>
+          <c:y val="0.416321616485238"/>
+          <c:w val="0.0914527376443245"/>
+          <c:h val="0.174904439729482"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2421,8 +2494,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2441,21 +2523,24 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.934230739270529E-2"/>
-          <c:y val="0.13237857639541298"/>
-          <c:w val="0.86752895981391298"/>
-          <c:h val="0.82988191717607018"/>
+          <c:x val="0.0993423073927053"/>
+          <c:y val="0.132378576395413"/>
+          <c:w val="0.867528959813913"/>
+          <c:h val="0.82988191717607"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2480,205 +2565,205 @@
                   <c:v>10.839</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.586999999999971</c:v>
+                  <c:v>19.58699999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19.586999999999971</c:v>
+                  <c:v>19.58699999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.586999999999971</c:v>
+                  <c:v>19.58699999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.343223499999954</c:v>
+                  <c:v>13.34322349999995</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.515253999999976</c:v>
+                  <c:v>13.51525399999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.870736000000022</c:v>
+                  <c:v>13.87073600000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14.241445999999968</c:v>
+                  <c:v>14.24144599999997</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>15.02854999999996</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>13.284393499999956</c:v>
+                  <c:v>13.28439349999996</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>13.397573999999979</c:v>
+                  <c:v>13.39757399999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>13.635295999999977</c:v>
+                  <c:v>13.63529599999998</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13.888165999999975</c:v>
+                  <c:v>13.88816599999998</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>14.439349999999973</c:v>
+                  <c:v>14.43934999999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.8829999999999991</c:v>
+                  <c:v>6.882999999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.9082102499999953</c:v>
+                  <c:v>6.908210249999995</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.9389810000000001</c:v>
+                  <c:v>6.938981</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.0172039999999987</c:v>
+                  <c:v>7.017203999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.1176689999999976</c:v>
+                  <c:v>7.117668999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.3853249999999857</c:v>
+                  <c:v>7.385324999999986</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>11.239000000000001</c:v>
+                  <c:v>11.239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2696,203 +2781,204 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00E+00">
-                  <c:v>4.8600000000000002E-5</c:v>
+                  <c:v>4.86E-5</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.5099999999999995E-4</c:v>
+                  <c:v>0.000551</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00E+00">
-                  <c:v>3.9899999999999996E-3</c:v>
+                  <c:v>0.00399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.29E-2</c:v>
+                  <c:v>0.0229</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00E+00">
-                  <c:v>1.9210000000000001E-4</c:v>
+                  <c:v>0.0001921</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0.00E+00">
-                  <c:v>5.1599999999999997E-4</c:v>
+                  <c:v>0.000516</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0.00E+00">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>1.686E-6</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>6.7000000000000002E-4</c:v>
+                  <c:v>0.00067</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>7.8300000000000002E-3</c:v>
+                  <c:v>0.00783</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>7.0140000000000003E-5</c:v>
+                  <c:v>7.014E-5</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>9.8269999999999998E-4</c:v>
+                  <c:v>0.0009827</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.8400000000000002E-2</c:v>
+                  <c:v>0.0284</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>5.4299999999999997E-6</c:v>
+                  <c:v>5.43E-6</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>3.5579999999999997E-4</c:v>
+                  <c:v>0.0003558</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>7.3499999999999998E-4</c:v>
+                  <c:v>0.000735</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>7.4799999999999997E-3</c:v>
+                  <c:v>0.00748</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>1.6099999999999998E-5</c:v>
+                  <c:v>1.61E-5</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>5.3660000000000003E-4</c:v>
+                  <c:v>0.0005366</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>4.1900000000000001E-3</c:v>
+                  <c:v>0.00419</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>9.0799999999999995E-3</c:v>
+                  <c:v>0.00908</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>1.7439999999999999E-6</c:v>
+                  <c:v>1.744E-6</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>7.8499999999999993E-3</c:v>
+                  <c:v>0.00785</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>7.6699999999999997E-3</c:v>
+                  <c:v>0.00767</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>4.2300000000000003E-3</c:v>
+                  <c:v>0.00423</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>7.9299999999999995E-3</c:v>
+                  <c:v>0.00793</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0699999999999999E-2</c:v>
+                  <c:v>0.0107</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>0.0165</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.01E-2</c:v>
+                  <c:v>0.0101</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>8.9200000000000008E-3</c:v>
+                  <c:v>0.00892</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>4.7000000000000002E-3</c:v>
+                  <c:v>0.0047</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>4.0600000000000002E-3</c:v>
+                  <c:v>0.00406</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>2.14E-3</c:v>
+                  <c:v>0.00214</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>2.2799999999999999E-3</c:v>
+                  <c:v>0.00228</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>2.7899999999999999E-3</c:v>
+                  <c:v>0.00279</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>5.5599999999999996E-4</c:v>
+                  <c:v>0.000556</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>4.1300000000000001E-4</c:v>
+                  <c:v>0.000413</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>4.26E-4</c:v>
+                  <c:v>0.000426</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>2.5399999999999999E-4</c:v>
+                  <c:v>0.000254</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>3.0899999999999998E-4</c:v>
+                  <c:v>0.000309</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>3.77E-4</c:v>
+                  <c:v>0.000377</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>2.5999999999999999E-3</c:v>
+                  <c:v>0.0026</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>4.1999999999999997E-3</c:v>
+                  <c:v>0.0042</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>0.0013</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>4.6999999999999999E-4</c:v>
+                  <c:v>0.00047</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>1.5999999999999999E-5</c:v>
+                  <c:v>1.6E-5</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>4.3000000000000002E-5</c:v>
+                  <c:v>4.3E-5</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>5.5000000000000003E-7</c:v>
+                  <c:v>5.5E-7</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>2.5000000000000002E-6</c:v>
+                  <c:v>2.5E-6</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.6E-3</c:v>
+                  <c:v>0.0076</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>4.96E-3</c:v>
+                  <c:v>0.00496</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>9.4800000000000006E-3</c:v>
+                  <c:v>0.00948</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>0.012</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>5.2900000000000004E-3</c:v>
+                  <c:v>0.00529</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>5.5399999999999998E-3</c:v>
+                  <c:v>0.00554</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>2.99E-3</c:v>
+                  <c:v>0.00299</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>8.0999999999999996E-3</c:v>
+                  <c:v>0.0081</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.6999999999999999E-3</c:v>
+                  <c:v>0.0017</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>1.49E-3</c:v>
+                  <c:v>0.00149</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.0499999999999999E-2</c:v>
+                  <c:v>0.0305</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.3100000000000003E-2</c:v>
+                  <c:v>0.0631</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.7499999999999999E-2</c:v>
+                  <c:v>0.0775</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>9.8199999999999996E-2</c:v>
+                  <c:v>0.0982</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>0.1226</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.14349999999999999</c:v>
+                  <c:v>0.1435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2912,22 +2998,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2939,20 +3025,21 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1.1400000000000001E-4</c:v>
+                  <c:v>0.000114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1200000000000005E-4</c:v>
+                  <c:v>0.000912</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8700000000000002E-3</c:v>
+                  <c:v>0.00687</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>0.017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2972,55 +3059,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.073470400000005</c:v>
+                  <c:v>17.07347040000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.174999999999979</c:v>
+                  <c:v>13.17499999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3032,82 +3119,95 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.4600000000000001E-5</c:v>
+                  <c:v>1.46E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.43E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0899999999999999E-4</c:v>
+                  <c:v>0.000709</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1399999999999996E-3</c:v>
+                  <c:v>0.00414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6400000000000002E-2</c:v>
+                  <c:v>0.0364</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0800000000000002E-5</c:v>
+                  <c:v>5.08E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5699999999999998E-3</c:v>
+                  <c:v>0.00357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1500000000000001E-3</c:v>
+                  <c:v>0.00615</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9399999999999992E-3</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>1.8700000000000001E-2</c:v>
+                  <c:v>0.0187</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>2.7300000000000001E-2</c:v>
+                  <c:v>0.0273</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>5.3900000000000003E-2</c:v>
+                  <c:v>0.0539</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>6.1199999999999997E-2</c:v>
+                  <c:v>0.0612</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>6.6199999999999995E-2</c:v>
+                  <c:v>0.0662</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>6.5199999999999994E-2</c:v>
+                  <c:v>0.0652</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>8.1299999999999997E-2</c:v>
+                  <c:v>0.0813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="46978944"/>
-        <c:axId val="46980480"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2130104008"/>
+        <c:axId val="2130107080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46978944"/>
+        <c:axId val="2130104008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46980480"/>
+        <c:crossAx val="2130107080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46980480"/>
+        <c:axId val="2130107080"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:txPr>
             <a:bodyPr rot="-5400000" vert="horz"/>
             <a:lstStyle/>
@@ -3120,8 +3220,10 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46978944"/>
+        <c:crossAx val="2130104008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3132,19 +3234,21 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.84885986899397015"/>
-          <c:y val="0.32342436989196616"/>
-          <c:w val="8.0835468241048203E-2"/>
-          <c:h val="0.17490443972948205"/>
+          <c:x val="0.84885986899397"/>
+          <c:y val="0.323424369891966"/>
+          <c:w val="0.0808354682410482"/>
+          <c:h val="0.174904439729482"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3535,21 +3639,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:CB134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:BW134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3210" topLeftCell="B1" activePane="topRight"/>
-      <selection activeCell="B12" sqref="B12"/>
-      <selection pane="topRight" activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <pane xSplit="4060" topLeftCell="J1" activePane="topRight"/>
+      <selection activeCell="B6" sqref="B6"/>
+      <selection pane="topRight" activeCell="U93" sqref="U93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:80">
+    <row r="2" spans="1:75">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3761,34 +3865,19 @@
         <v>44</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BW2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BX2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BY2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BZ2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CA2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CB2" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:80">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -4000,34 +4089,19 @@
         <v>2006</v>
       </c>
       <c r="BT3">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="BU3">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="BV3">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="BW3">
-        <v>2008</v>
-      </c>
-      <c r="BX3">
-        <v>2008</v>
-      </c>
-      <c r="BY3">
-        <v>2008</v>
-      </c>
-      <c r="BZ3">
         <v>2006</v>
       </c>
-      <c r="CA3">
-        <v>2006</v>
-      </c>
-      <c r="CB3">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:80">
+    </row>
+    <row r="4" spans="1:75">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -4235,8 +4309,20 @@
       <c r="BS4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:80" s="4" customFormat="1">
+      <c r="BT4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" s="4" customFormat="1">
       <c r="B5" s="4" t="s">
         <v>96</v>
       </c>
@@ -4448,25 +4534,19 @@
         <v>270</v>
       </c>
       <c r="BT5" s="4">
-        <v>13</v>
+        <v>25.5</v>
       </c>
       <c r="BU5" s="4">
-        <v>17.600000000000001</v>
+        <v>25.5</v>
       </c>
       <c r="BV5" s="4">
-        <v>34.4</v>
+        <v>25.5</v>
       </c>
       <c r="BW5" s="4">
-        <v>55.6</v>
-      </c>
-      <c r="BX5" s="4">
-        <v>85</v>
-      </c>
-      <c r="BY5" s="4">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:80" s="4" customFormat="1">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75" s="4" customFormat="1">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -4645,25 +4725,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="BT6" s="4">
-        <v>2</v>
+        <v>1.48</v>
       </c>
       <c r="BU6" s="4">
-        <v>1.8</v>
+        <v>1.48</v>
       </c>
       <c r="BV6" s="4">
-        <v>2.1</v>
+        <v>1.48</v>
       </c>
       <c r="BW6" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="BX6" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="BY6" s="4">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:80" s="4" customFormat="1">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" s="4" customFormat="1">
       <c r="B7" s="4" t="s">
         <v>97</v>
       </c>
@@ -4869,34 +4943,19 @@
         <v>74</v>
       </c>
       <c r="BT7" s="4">
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="BU7" s="4">
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="BV7" s="4">
-        <v>97</v>
+        <v>98.5</v>
       </c>
       <c r="BW7" s="4">
-        <v>97</v>
-      </c>
-      <c r="BX7" s="4">
-        <v>97</v>
-      </c>
-      <c r="BY7" s="4">
-        <v>97</v>
-      </c>
-      <c r="BZ7" s="4">
         <v>98.5</v>
       </c>
-      <c r="CA7" s="4">
-        <v>98.5</v>
-      </c>
-      <c r="CB7" s="4">
-        <v>98.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:80" s="5" customFormat="1">
+    </row>
+    <row r="8" spans="1:75" s="5" customFormat="1">
       <c r="B8" s="5" t="s">
         <v>114</v>
       </c>
@@ -5083,17 +5142,20 @@
       <c r="BS8" s="5">
         <v>10</v>
       </c>
-      <c r="BZ8" s="5">
+      <c r="BT8" s="5">
         <v>1</v>
       </c>
-      <c r="CA8" s="5">
+      <c r="BU8" s="5">
         <v>1</v>
       </c>
-      <c r="CB8" s="5">
+      <c r="BV8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:80" s="5" customFormat="1">
+      <c r="BW8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" s="5" customFormat="1">
       <c r="B9" s="5" t="s">
         <v>115</v>
       </c>
@@ -5305,34 +5367,19 @@
         <v>73</v>
       </c>
       <c r="BT9" s="5" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="BU9" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="BV9" s="5" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="BW9" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="BX9" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="BY9" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="BZ9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="CA9" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="CB9" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:80" s="5" customFormat="1">
+    </row>
+    <row r="10" spans="1:75" s="5" customFormat="1">
       <c r="B10" s="5" t="s">
         <v>116</v>
       </c>
@@ -5382,7 +5429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:80" s="5" customFormat="1">
+    <row r="11" spans="1:75" s="5" customFormat="1">
       <c r="B11" s="5" t="s">
         <v>117</v>
       </c>
@@ -5432,7 +5479,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="12" spans="1:80" s="5" customFormat="1">
+    <row r="12" spans="1:75" s="5" customFormat="1">
       <c r="B12" s="5" t="s">
         <v>87</v>
       </c>
@@ -5712,17 +5759,24 @@
         <f t="shared" si="1"/>
         <v>487</v>
       </c>
-      <c r="BZ12" s="5">
-        <v>61</v>
-      </c>
-      <c r="CA12" s="5">
-        <v>138.30000000000001</v>
-      </c>
-      <c r="CB12" s="5">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:80" s="14" customFormat="1">
+      <c r="BT12" s="5">
+        <f t="shared" ref="BT12:BV12" si="2">IF(ISBLANK(BT10),LOOKUP(BT9,$A$100:$A$108,$F$100:$F$108),BT11*LOOKUP(BT9,$A$100:$A$108,$F$100:$F$108)+(1-BT11)*LOOKUP(BT10,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="BU12" s="5">
+        <f t="shared" si="2"/>
+        <v>411</v>
+      </c>
+      <c r="BV12" s="5">
+        <f t="shared" si="2"/>
+        <v>487</v>
+      </c>
+      <c r="BW12" s="5">
+        <f t="shared" ref="BW12" si="3">IF(ISBLANK(BW10),LOOKUP(BW9,$A$100:$A$108,$F$100:$F$108),BW11*LOOKUP(BW9,$A$100:$A$108,$F$100:$F$108)+(1-BW11)*LOOKUP(BW10,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:75" s="14" customFormat="1">
       <c r="B13" s="14" t="s">
         <v>98</v>
       </c>
@@ -5731,7 +5785,7 @@
         <v>10.839</v>
       </c>
       <c r="D13" s="14">
-        <f t="shared" ref="D13:BO13" si="2">IF(ISBLANK(D10), 4*(LOOKUP(D9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D11*LOOKUP(D9,$A$101:$A$108,$B$101:$B$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D11*LOOKUP(D9,$A$101:$A$108,$C$101:$C$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D11*LOOKUP(D9,$A$101:$A$108,$D$101:$D$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D13:BO13" si="4">IF(ISBLANK(D10), 4*(LOOKUP(D9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D11*LOOKUP(D9,$A$101:$A$108,$B$101:$B$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D11*LOOKUP(D9,$A$101:$A$108,$C$101:$C$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D11*LOOKUP(D9,$A$101:$A$108,$D$101:$D$108)+(1-D11)*LOOKUP(D10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>10.839</v>
       </c>
       <c r="E13" s="14">
@@ -5743,267 +5797,283 @@
         <v>13.174999999999979</v>
       </c>
       <c r="G13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="H13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="J13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="K13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="L13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="M13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="N13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="O13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="P13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="Q13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19.586999999999971</v>
       </c>
       <c r="R13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19.586999999999971</v>
       </c>
       <c r="S13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19.586999999999971</v>
       </c>
       <c r="T13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="U13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="V13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="W13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="X13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="Y13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="Z13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AA13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AB13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AC13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AD13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AE13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AF13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.343223499999954</v>
       </c>
       <c r="AG13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.515253999999976</v>
       </c>
       <c r="AH13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.870736000000022</v>
       </c>
       <c r="AI13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14.241445999999968</v>
       </c>
       <c r="AJ13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15.02854999999996</v>
       </c>
       <c r="AK13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.284393499999956</v>
       </c>
       <c r="AL13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.397573999999979</v>
       </c>
       <c r="AM13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.635295999999977</v>
       </c>
       <c r="AN13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.888165999999975</v>
       </c>
       <c r="AO13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14.439349999999973</v>
       </c>
       <c r="AP13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.8829999999999991</v>
       </c>
       <c r="AQ13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.9082102499999953</v>
       </c>
       <c r="AR13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.9389810000000001</v>
       </c>
       <c r="AS13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.0172039999999987</v>
       </c>
       <c r="AT13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.1176689999999976</v>
       </c>
       <c r="AU13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.3853249999999857</v>
       </c>
       <c r="AV13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AW13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AX13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AY13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="AZ13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BA13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BB13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BC13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BD13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BE13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BF13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BG13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BH13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BI13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BJ13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BK13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13.174999999999979</v>
       </c>
       <c r="BL13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BM13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BN13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BO13" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BP13" s="14">
-        <f t="shared" ref="BP13:BS13" si="3">IF(ISBLANK(BP10), 4*(LOOKUP(BP9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(BP9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(BP9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((BP11*LOOKUP(BP9,$A$101:$A$108,$B$101:$B$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((BP11*LOOKUP(BP9,$A$101:$A$108,$C$101:$C$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((BP11*LOOKUP(BP9,$A$101:$A$108,$D$101:$D$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="BP13:BR13" si="5">IF(ISBLANK(BP10), 4*(LOOKUP(BP9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(BP9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(BP9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((BP11*LOOKUP(BP9,$A$101:$A$108,$B$101:$B$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((BP11*LOOKUP(BP9,$A$101:$A$108,$C$101:$C$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((BP11*LOOKUP(BP9,$A$101:$A$108,$D$101:$D$108)+(1-BP11)*LOOKUP(BP10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>11.239000000000001</v>
       </c>
       <c r="BQ13" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BR13" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11.239000000000001</v>
       </c>
       <c r="BS13" s="14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(BS10), 4*(LOOKUP(BS9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(BS9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(BS9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((BS11*LOOKUP(BS9,$A$101:$A$108,$B$101:$B$108)+(1-BS11)*LOOKUP(BS10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((BS11*LOOKUP(BS9,$A$101:$A$108,$C$101:$C$108)+(1-BS11)*LOOKUP(BS10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((BS11*LOOKUP(BS9,$A$101:$A$108,$D$101:$D$108)+(1-BS11)*LOOKUP(BS10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>11.239000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:80" s="5" customFormat="1">
+      <c r="BT13" s="14">
+        <f t="shared" ref="BT13:BV13" si="6">IF(ISBLANK(BT10), 4*(LOOKUP(BT9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(BT9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(BT9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((BT11*LOOKUP(BT9,$A$101:$A$108,$B$101:$B$108)+(1-BT11)*LOOKUP(BT10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((BT11*LOOKUP(BT9,$A$101:$A$108,$C$101:$C$108)+(1-BT11)*LOOKUP(BT10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((BT11*LOOKUP(BT9,$A$101:$A$108,$D$101:$D$108)+(1-BT11)*LOOKUP(BT10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <v>13.174999999999979</v>
+      </c>
+      <c r="BU13" s="14">
+        <f t="shared" si="6"/>
+        <v>19.586999999999971</v>
+      </c>
+      <c r="BV13" s="14">
+        <f t="shared" si="6"/>
+        <v>11.239000000000001</v>
+      </c>
+      <c r="BW13" s="14">
+        <f t="shared" ref="BW13" si="7">IF(ISBLANK(BW10), 4*(LOOKUP(BW9,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(BW9,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(BW9,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((BW11*LOOKUP(BW9,$A$101:$A$108,$B$101:$B$108)+(1-BW11)*LOOKUP(BW10,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((BW11*LOOKUP(BW9,$A$101:$A$108,$C$101:$C$108)+(1-BW11)*LOOKUP(BW10,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((BW11*LOOKUP(BW9,$A$101:$A$108,$D$101:$D$108)+(1-BW11)*LOOKUP(BW10,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <v>13.174999999999979</v>
+      </c>
+    </row>
+    <row r="14" spans="1:75" s="5" customFormat="1">
       <c r="B14" s="5" t="s">
         <v>99</v>
       </c>
@@ -6056,7 +6126,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:80" s="5" customFormat="1">
+    <row r="15" spans="1:75" s="5" customFormat="1">
       <c r="B15" s="5" t="s">
         <v>100</v>
       </c>
@@ -6187,7 +6257,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:80" s="5" customFormat="1">
+    <row r="16" spans="1:75" s="5" customFormat="1">
       <c r="B16" s="5" t="s">
         <v>101</v>
       </c>
@@ -6318,7 +6388,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="2:80" s="6" customFormat="1">
+    <row r="17" spans="2:75" s="6" customFormat="1">
       <c r="B17" s="6" t="s">
         <v>102</v>
       </c>
@@ -6478,8 +6548,11 @@
       <c r="BS17" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="2:80" s="7" customFormat="1">
+      <c r="BW17" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:75" s="7" customFormat="1">
       <c r="B18" s="7" t="s">
         <v>103</v>
       </c>
@@ -6690,26 +6763,8 @@
       <c r="BS18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="BT18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="BU18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="BV18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="BW18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="BX18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="BY18" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:80" s="7" customFormat="1">
+    </row>
+    <row r="19" spans="2:75" s="7" customFormat="1">
       <c r="B19" s="7" t="s">
         <v>104</v>
       </c>
@@ -6890,17 +6945,20 @@
       <c r="BS19" s="7">
         <v>1500</v>
       </c>
-      <c r="BZ19" s="7">
+      <c r="BT19" s="7">
         <v>4000</v>
       </c>
-      <c r="CA19" s="7">
+      <c r="BU19" s="7">
         <v>4000</v>
       </c>
-      <c r="CB19" s="7">
+      <c r="BV19" s="7">
         <v>4000</v>
       </c>
-    </row>
-    <row r="20" spans="2:80" s="7" customFormat="1">
+      <c r="BW19" s="7">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:75" s="7" customFormat="1">
       <c r="B20" s="7" t="s">
         <v>105</v>
       </c>
@@ -6973,17 +7031,20 @@
       <c r="AU20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="BZ20" s="7" t="s">
+      <c r="BT20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="CA20" s="7">
+      <c r="BU20" s="7">
         <v>60</v>
       </c>
-      <c r="CB20" s="7">
+      <c r="BV20" s="7">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="2:80" s="7" customFormat="1">
+      <c r="BW20" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="2:75" s="7" customFormat="1">
       <c r="B21" s="7" t="s">
         <v>106</v>
       </c>
@@ -7138,34 +7199,19 @@
         <v>35</v>
       </c>
       <c r="BT21" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BU21" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BV21" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BW21" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="BX21" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="BY21" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="BZ21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="CA21" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="CB21" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="2:80">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:75">
       <c r="B22" t="s">
         <v>107</v>
       </c>
@@ -7238,26 +7284,8 @@
       <c r="BS22" s="12">
         <v>100</v>
       </c>
-      <c r="BT22" s="12">
-        <v>140</v>
-      </c>
-      <c r="BU22" s="12">
-        <v>140</v>
-      </c>
-      <c r="BV22" s="12">
-        <v>140</v>
-      </c>
-      <c r="BW22" s="12">
-        <v>150</v>
-      </c>
-      <c r="BX22" s="12">
-        <v>150</v>
-      </c>
-      <c r="BY22" s="12">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="2:80">
+    </row>
+    <row r="23" spans="2:75">
       <c r="B23" t="s">
         <v>108</v>
       </c>
@@ -7334,26 +7362,8 @@
       <c r="BS23" s="12">
         <v>10</v>
       </c>
-      <c r="BT23" s="12">
-        <v>2</v>
-      </c>
-      <c r="BU23" s="12">
-        <v>2</v>
-      </c>
-      <c r="BV23" s="12">
-        <v>2</v>
-      </c>
-      <c r="BW23" s="12">
-        <v>2</v>
-      </c>
-      <c r="BX23" s="12">
-        <v>2</v>
-      </c>
-      <c r="BY23" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:80">
+    </row>
+    <row r="24" spans="2:75">
       <c r="B24" t="s">
         <v>109</v>
       </c>
@@ -7380,7 +7390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:80" s="8" customFormat="1">
+    <row r="25" spans="2:75" s="8" customFormat="1">
       <c r="B25" s="8" t="s">
         <v>110</v>
       </c>
@@ -7592,34 +7602,19 @@
         <v>4</v>
       </c>
       <c r="BT25" s="8" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="BU25" s="8" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="BV25" s="8" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="BW25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="BX25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="BY25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="BZ25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="CA25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="CB25" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:80" s="8" customFormat="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:75" s="8" customFormat="1">
       <c r="B26" s="8" t="s">
         <v>120</v>
       </c>
@@ -7830,8 +7825,20 @@
       <c r="BS26" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="2:80" s="8" customFormat="1">
+      <c r="BT26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BU26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BV26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW26" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="2:75" s="8" customFormat="1">
       <c r="B27" s="8" t="s">
         <v>121</v>
       </c>
@@ -8036,8 +8043,20 @@
       <c r="BS27" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="2:80" s="8" customFormat="1">
+      <c r="BT27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="BU27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="BV27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="BW27" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:75" s="8" customFormat="1">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
@@ -8089,8 +8108,14 @@
       <c r="BS28" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="2:80" s="8" customFormat="1">
+      <c r="BT28" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="BW28" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="2:75" s="8" customFormat="1">
       <c r="B29" s="8" t="s">
         <v>112</v>
       </c>
@@ -8143,7 +8168,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:80" s="8" customFormat="1">
+    <row r="30" spans="2:75" s="8" customFormat="1">
       <c r="B30" s="8" t="s">
         <v>113</v>
       </c>
@@ -8349,34 +8374,19 @@
         <v>0.14349999999999999</v>
       </c>
       <c r="BT30" s="9">
-        <v>2.0000000000000001E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="BU30" s="9">
-        <v>2.0000000000000001E-4</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="BV30" s="9">
-        <v>4.0000000000000003E-5</v>
+        <v>2.3E-2</v>
       </c>
       <c r="BW30" s="9">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="BX30" s="9">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="BY30" s="9">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="BZ30" s="9">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="CA30" s="9">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="CB30" s="9">
-        <v>2.3E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:80">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:75">
       <c r="C31">
         <v>1</v>
       </c>
@@ -8385,299 +8395,291 @@
         <v>2</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E31:BP31" si="4">D31+1</f>
+        <f t="shared" ref="E31:BP31" si="8">D31+1</f>
         <v>3</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="I31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="J31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="K31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="L31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="M31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="N31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="O31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="P31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="R31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="S31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="T31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="U31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="V31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="W31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="X31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
       <c r="AH31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="AI31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="AJ31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
       <c r="AK31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="AL31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="AM31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="AN31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="AO31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
       <c r="AP31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="AQ31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
       <c r="AR31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
       <c r="AS31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>43</v>
       </c>
       <c r="AT31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="AU31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="AV31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
       <c r="AW31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="AX31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
       <c r="AY31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>49</v>
       </c>
       <c r="AZ31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="BA31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>51</v>
       </c>
       <c r="BB31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>52</v>
       </c>
       <c r="BC31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>53</v>
       </c>
       <c r="BD31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>54</v>
       </c>
       <c r="BE31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="BF31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="BG31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="BH31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
       <c r="BI31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
       <c r="BJ31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="BK31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>61</v>
       </c>
       <c r="BL31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>62</v>
       </c>
       <c r="BM31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
       <c r="BN31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="BO31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="BP31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>66</v>
       </c>
       <c r="BQ31">
-        <f t="shared" ref="BQ31:BS31" si="5">BP31+1</f>
+        <f t="shared" ref="BQ31:BS31" si="9">BP31+1</f>
         <v>67</v>
       </c>
       <c r="BR31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
       <c r="BS31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>69</v>
       </c>
       <c r="BT31">
-        <f t="shared" ref="BT31" si="6">BS31+1</f>
+        <f t="shared" ref="BT31" si="10">BS31+1</f>
         <v>70</v>
       </c>
       <c r="BU31">
-        <f t="shared" ref="BU31" si="7">BT31+1</f>
+        <f t="shared" ref="BU31" si="11">BT31+1</f>
         <v>71</v>
       </c>
       <c r="BV31">
-        <f t="shared" ref="BV31" si="8">BU31+1</f>
+        <f t="shared" ref="BV31:BW31" si="12">BU31+1</f>
         <v>72</v>
       </c>
       <c r="BW31">
-        <f t="shared" ref="BW31" si="9">BV31+1</f>
+        <f t="shared" si="12"/>
         <v>73</v>
       </c>
-      <c r="BX31">
-        <f t="shared" ref="BX31" si="10">BW31+1</f>
-        <v>74</v>
-      </c>
-      <c r="BY31">
-        <f t="shared" ref="BY31" si="11">BX31+1</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="2:80" s="2" customFormat="1" ht="78" customHeight="1">
+    </row>
+    <row r="32" spans="2:75" s="2" customFormat="1" ht="78" customHeight="1">
       <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
@@ -8723,13 +8725,13 @@
         <v>14</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -8923,7 +8925,7 @@
         <v>22</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>73</v>
@@ -8948,23 +8950,23 @@
         <v>334</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" ref="D44:E44" si="12">IF(ISBLANK(D42),LOOKUP(D41,$A$100:$A$108,$F$100:$F$108),D43*LOOKUP(D41,$A$100:$A$108,$F$100:$F$108)+(1-D43)*LOOKUP(D42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="D44:E44" si="13">IF(ISBLANK(D42),LOOKUP(D41,$A$100:$A$108,$F$100:$F$108),D43*LOOKUP(D41,$A$100:$A$108,$F$100:$F$108)+(1-D43)*LOOKUP(D42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="12"/>
-        <v>334</v>
-      </c>
-      <c r="F44" s="5">
-        <f t="shared" ref="F44:G44" si="13">IF(ISBLANK(F42),LOOKUP(F41,$A$100:$A$108,$F$100:$F$108),F43*LOOKUP(F41,$A$100:$A$108,$F$100:$F$108)+(1-F43)*LOOKUP(F42,$A$100:$A$108,$F$100:$F$108))</f>
-        <v>334</v>
-      </c>
-      <c r="G44" s="5">
         <f t="shared" si="13"/>
         <v>334</v>
       </c>
+      <c r="F44" s="5">
+        <f t="shared" ref="F44:G44" si="14">IF(ISBLANK(F42),LOOKUP(F41,$A$100:$A$108,$F$100:$F$108),F43*LOOKUP(F41,$A$100:$A$108,$F$100:$F$108)+(1-F43)*LOOKUP(F42,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="G44" s="5">
+        <f t="shared" si="14"/>
+        <v>334</v>
+      </c>
       <c r="H44" s="5">
-        <f t="shared" ref="H44" si="14">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="H44" si="15">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
     </row>
@@ -8977,23 +8979,23 @@
         <v>13.174999999999979</v>
       </c>
       <c r="D45" s="14">
-        <f t="shared" ref="D45:H45" si="15">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D45:H45" si="16">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>13.174999999999979</v>
       </c>
       <c r="E45" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13.174999999999979</v>
       </c>
       <c r="F45" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13.174999999999979</v>
       </c>
       <c r="G45" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13.174999999999979</v>
       </c>
       <c r="H45" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13.174999999999979</v>
       </c>
     </row>
@@ -9104,13 +9106,13 @@
         <v>25</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="2:11">
@@ -9154,10 +9156,10 @@
         <v>4</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:11" s="8" customFormat="1">
@@ -9244,28 +9246,40 @@
     </row>
     <row r="62" spans="2:11">
       <c r="C62">
-        <f>BS31+1</f>
-        <v>70</v>
+        <f>BW31+1</f>
+        <v>74</v>
       </c>
       <c r="D62">
         <f>C62+1</f>
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:H62" si="16">D62+1</f>
-        <v>72</v>
+        <f t="shared" ref="E62:H62" si="17">D62+1</f>
+        <v>76</v>
       </c>
       <c r="F62">
-        <f t="shared" si="16"/>
-        <v>73</v>
+        <f t="shared" si="17"/>
+        <v>77</v>
       </c>
       <c r="G62">
-        <f t="shared" si="16"/>
-        <v>74</v>
+        <f t="shared" si="17"/>
+        <v>78</v>
       </c>
       <c r="H62">
-        <f t="shared" si="16"/>
-        <v>75</v>
+        <f t="shared" si="17"/>
+        <v>79</v>
+      </c>
+      <c r="I62">
+        <f t="shared" ref="I62" si="18">H62+1</f>
+        <v>80</v>
+      </c>
+      <c r="J62">
+        <f t="shared" ref="J62" si="19">I62+1</f>
+        <v>81</v>
+      </c>
+      <c r="K62">
+        <f t="shared" ref="K62" si="20">J62+1</f>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="2:11">
@@ -9332,13 +9346,13 @@
         <v>44</v>
       </c>
       <c r="T65" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:22">
@@ -9754,7 +9768,7 @@
         <v>22</v>
       </c>
       <c r="U72" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>73</v>
@@ -9815,67 +9829,67 @@
         <v>334.88</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" ref="D75:E75" si="17">IF(ISBLANK(D73),LOOKUP(D72,$A$100:$A$108,$F$100:$F$108),D74*LOOKUP(D72,$A$100:$A$108,$F$100:$F$108)+(1-D74)*LOOKUP(D73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="D75:E75" si="21">IF(ISBLANK(D73),LOOKUP(D72,$A$100:$A$108,$F$100:$F$108),D74*LOOKUP(D72,$A$100:$A$108,$F$100:$F$108)+(1-D74)*LOOKUP(D73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>334.88</v>
       </c>
       <c r="F75" s="5">
-        <f t="shared" ref="F75:G75" si="18">IF(ISBLANK(F73),LOOKUP(F72,$A$100:$A$108,$F$100:$F$108),F74*LOOKUP(F72,$A$100:$A$108,$F$100:$F$108)+(1-F74)*LOOKUP(F73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="F75:G75" si="22">IF(ISBLANK(F73),LOOKUP(F72,$A$100:$A$108,$F$100:$F$108),F74*LOOKUP(F72,$A$100:$A$108,$F$100:$F$108)+(1-F74)*LOOKUP(F73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="G75" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>334.88</v>
       </c>
       <c r="H75" s="5">
-        <f t="shared" ref="H75:I75" si="19">IF(ISBLANK(H73),LOOKUP(H72,$A$100:$A$108,$F$100:$F$108),H74*LOOKUP(H72,$A$100:$A$108,$F$100:$F$108)+(1-H74)*LOOKUP(H73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="H75:I75" si="23">IF(ISBLANK(H73),LOOKUP(H72,$A$100:$A$108,$F$100:$F$108),H74*LOOKUP(H72,$A$100:$A$108,$F$100:$F$108)+(1-H74)*LOOKUP(H73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334.88</v>
       </c>
       <c r="I75" s="5">
-        <f t="shared" si="19"/>
-        <v>334</v>
-      </c>
-      <c r="J75" s="5">
-        <f t="shared" ref="J75:K75" si="20">IF(ISBLANK(J73),LOOKUP(J72,$A$100:$A$108,$F$100:$F$108),J74*LOOKUP(J72,$A$100:$A$108,$F$100:$F$108)+(1-J74)*LOOKUP(J73,$A$100:$A$108,$F$100:$F$108))</f>
-        <v>334</v>
-      </c>
-      <c r="K75" s="5">
-        <f t="shared" si="20"/>
-        <v>334</v>
-      </c>
-      <c r="L75" s="5">
-        <f t="shared" ref="L75:M75" si="21">IF(ISBLANK(L73),LOOKUP(L72,$A$100:$A$108,$F$100:$F$108),L74*LOOKUP(L72,$A$100:$A$108,$F$100:$F$108)+(1-L74)*LOOKUP(L73,$A$100:$A$108,$F$100:$F$108))</f>
-        <v>334</v>
-      </c>
-      <c r="M75" s="5">
-        <f t="shared" si="21"/>
-        <v>334</v>
-      </c>
-      <c r="N75" s="5">
-        <f t="shared" ref="N75:O75" si="22">IF(ISBLANK(N73),LOOKUP(N72,$A$100:$A$108,$F$100:$F$108),N74*LOOKUP(N72,$A$100:$A$108,$F$100:$F$108)+(1-N74)*LOOKUP(N73,$A$100:$A$108,$F$100:$F$108))</f>
-        <v>334</v>
-      </c>
-      <c r="O75" s="5">
-        <f t="shared" si="22"/>
-        <v>334</v>
-      </c>
-      <c r="P75" s="5">
-        <f t="shared" ref="P75:Q75" si="23">IF(ISBLANK(P73),LOOKUP(P72,$A$100:$A$108,$F$100:$F$108),P74*LOOKUP(P72,$A$100:$A$108,$F$100:$F$108)+(1-P74)*LOOKUP(P73,$A$100:$A$108,$F$100:$F$108))</f>
-        <v>334</v>
-      </c>
-      <c r="Q75" s="5">
         <f t="shared" si="23"/>
         <v>334</v>
       </c>
+      <c r="J75" s="5">
+        <f t="shared" ref="J75:K75" si="24">IF(ISBLANK(J73),LOOKUP(J72,$A$100:$A$108,$F$100:$F$108),J74*LOOKUP(J72,$A$100:$A$108,$F$100:$F$108)+(1-J74)*LOOKUP(J73,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="K75" s="5">
+        <f t="shared" si="24"/>
+        <v>334</v>
+      </c>
+      <c r="L75" s="5">
+        <f t="shared" ref="L75:M75" si="25">IF(ISBLANK(L73),LOOKUP(L72,$A$100:$A$108,$F$100:$F$108),L74*LOOKUP(L72,$A$100:$A$108,$F$100:$F$108)+(1-L74)*LOOKUP(L73,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="M75" s="5">
+        <f t="shared" si="25"/>
+        <v>334</v>
+      </c>
+      <c r="N75" s="5">
+        <f t="shared" ref="N75:O75" si="26">IF(ISBLANK(N73),LOOKUP(N72,$A$100:$A$108,$F$100:$F$108),N74*LOOKUP(N72,$A$100:$A$108,$F$100:$F$108)+(1-N74)*LOOKUP(N73,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="O75" s="5">
+        <f t="shared" si="26"/>
+        <v>334</v>
+      </c>
+      <c r="P75" s="5">
+        <f t="shared" ref="P75:Q75" si="27">IF(ISBLANK(P73),LOOKUP(P72,$A$100:$A$108,$F$100:$F$108),P74*LOOKUP(P72,$A$100:$A$108,$F$100:$F$108)+(1-P74)*LOOKUP(P73,$A$100:$A$108,$F$100:$F$108))</f>
+        <v>334</v>
+      </c>
+      <c r="Q75" s="5">
+        <f t="shared" si="27"/>
+        <v>334</v>
+      </c>
       <c r="R75" s="5">
-        <f t="shared" ref="R75:S75" si="24">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="R75:S75" si="28">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="S75" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>334</v>
       </c>
     </row>
@@ -9888,67 +9902,67 @@
         <v>17.073470400000005</v>
       </c>
       <c r="D76" s="14">
-        <f t="shared" ref="D76:S76" si="25">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D76:S76" si="29">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>17.073470400000005</v>
       </c>
       <c r="E76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>17.073470400000005</v>
       </c>
       <c r="F76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>17.073470400000005</v>
       </c>
       <c r="G76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>17.073470400000005</v>
       </c>
       <c r="H76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>17.073470400000005</v>
       </c>
       <c r="I76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="K76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="L76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="M76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="N76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="O76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="P76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="Q76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="R76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
       <c r="S76" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>13.174999999999979</v>
       </c>
     </row>
@@ -10257,13 +10271,13 @@
         <v>35</v>
       </c>
       <c r="T83" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:22">
@@ -10637,72 +10651,84 @@
     </row>
     <row r="93" spans="1:22">
       <c r="C93">
-        <f>H62+1</f>
-        <v>76</v>
+        <f>K62+1</f>
+        <v>83</v>
       </c>
       <c r="D93">
         <f>C93+1</f>
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E93">
-        <f t="shared" ref="E93:S93" si="26">D93+1</f>
-        <v>78</v>
+        <f t="shared" ref="E93:S93" si="30">D93+1</f>
+        <v>85</v>
       </c>
       <c r="F93">
-        <f t="shared" si="26"/>
-        <v>79</v>
+        <f t="shared" si="30"/>
+        <v>86</v>
       </c>
       <c r="G93">
-        <f t="shared" si="26"/>
-        <v>80</v>
+        <f t="shared" si="30"/>
+        <v>87</v>
       </c>
       <c r="H93">
-        <f t="shared" si="26"/>
-        <v>81</v>
+        <f t="shared" si="30"/>
+        <v>88</v>
       </c>
       <c r="I93">
-        <f t="shared" si="26"/>
-        <v>82</v>
+        <f t="shared" si="30"/>
+        <v>89</v>
       </c>
       <c r="J93">
-        <f t="shared" si="26"/>
-        <v>83</v>
+        <f t="shared" si="30"/>
+        <v>90</v>
       </c>
       <c r="K93">
-        <f t="shared" si="26"/>
-        <v>84</v>
+        <f t="shared" si="30"/>
+        <v>91</v>
       </c>
       <c r="L93">
-        <f t="shared" si="26"/>
-        <v>85</v>
+        <f t="shared" si="30"/>
+        <v>92</v>
       </c>
       <c r="M93">
-        <f t="shared" si="26"/>
-        <v>86</v>
+        <f t="shared" si="30"/>
+        <v>93</v>
       </c>
       <c r="N93">
-        <f t="shared" si="26"/>
-        <v>87</v>
+        <f t="shared" si="30"/>
+        <v>94</v>
       </c>
       <c r="O93">
-        <f t="shared" si="26"/>
-        <v>88</v>
+        <f t="shared" si="30"/>
+        <v>95</v>
       </c>
       <c r="P93">
-        <f t="shared" si="26"/>
-        <v>89</v>
+        <f t="shared" si="30"/>
+        <v>96</v>
       </c>
       <c r="Q93">
-        <f t="shared" si="26"/>
-        <v>90</v>
+        <f t="shared" si="30"/>
+        <v>97</v>
       </c>
       <c r="R93">
-        <f t="shared" si="26"/>
-        <v>91</v>
+        <f t="shared" si="30"/>
+        <v>98</v>
       </c>
       <c r="S93">
-        <f t="shared" si="26"/>
-        <v>92</v>
+        <f t="shared" si="30"/>
+        <v>99</v>
+      </c>
+      <c r="T93">
+        <f t="shared" ref="T93" si="31">S93+1</f>
+        <v>100</v>
+      </c>
+      <c r="U93">
+        <f t="shared" ref="U93" si="32">T93+1</f>
+        <v>101</v>
+      </c>
+      <c r="V93">
+        <f t="shared" ref="V93" si="33">U93+1</f>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:22">
@@ -11051,12 +11077,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11068,12 +11094,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
no changes i don't want this
blah
</commit_message>
<xml_diff>
--- a/OFET fab table copy.xlsx
+++ b/OFET fab table copy.xlsx
@@ -1534,11 +1534,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2123955384"/>
-        <c:axId val="2122509480"/>
+        <c:axId val="2083834360"/>
+        <c:axId val="2036440792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2123955384"/>
+        <c:axId val="2083834360"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1575,12 +1575,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122509480"/>
+        <c:crossAx val="2036440792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122509480"/>
+        <c:axId val="2036440792"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1610,7 +1610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123955384"/>
+        <c:crossAx val="2083834360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2291,11 +2291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124001400"/>
-        <c:axId val="2124004392"/>
+        <c:axId val="2036351544"/>
+        <c:axId val="2036348552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124001400"/>
+        <c:axId val="2036351544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,12 +2305,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124004392"/>
+        <c:crossAx val="2036348552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124004392"/>
+        <c:axId val="2036348552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2345,7 +2345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124001400"/>
+        <c:crossAx val="2036351544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2406,6 +2406,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3062,11 +3063,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124040824"/>
-        <c:axId val="2124043816"/>
+        <c:axId val="2126843352"/>
+        <c:axId val="2126846344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124040824"/>
+        <c:axId val="2126843352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3076,12 +3077,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124043816"/>
+        <c:crossAx val="2126846344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124043816"/>
+        <c:axId val="2126846344"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3089,6 +3090,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:txPr>
             <a:bodyPr rot="-5400000" vert="horz"/>
@@ -3105,7 +3107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124040824"/>
+        <c:crossAx val="2126843352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3122,6 +3124,432 @@
           <c:h val="0.174904439729482"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AP$13:$AU$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.882999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.908210249999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.938981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.017203999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.117668999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.385324999999986</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AP$30:$AU$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.000556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000413</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000426</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000254</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000309</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2081968664"/>
+        <c:axId val="2128335704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2081968664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128335704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2128335704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2081968664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$13:$AO$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13.28439349999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.39757399999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.63529599999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.88816599999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.43934999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$30:$AO$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00406</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00214</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2131520248"/>
+        <c:axId val="2131173816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2131520248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131173816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2131173816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131520248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AE$13:$AJ$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13.17499999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.34322349999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.51525399999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.87073600000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.24144599999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.02854999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AE$30:$AJ$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.00423</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00793</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.0107</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.0165</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.0101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00892</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2133691608"/>
+        <c:axId val="2133364584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2133691608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2133364584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2133364584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2133691608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3227,6 +3655,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>514350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>450850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3524,10 +4042,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BW134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4060" activePane="topRight"/>
-      <selection activeCell="A17" sqref="A17:XFD17"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="4060" topLeftCell="Z1" activePane="topRight"/>
+      <selection activeCell="B3" sqref="B3:B30"/>
+      <selection pane="topRight" activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Cleaner, more readable functions
XL2STRUCT
Struct2Data
Run_Regress

All have functional inputs and outputs, and the permutations in
Run_Regress are now controlled by an input argument
</commit_message>
<xml_diff>
--- a/OFET fab table copy.xlsx
+++ b/OFET fab table copy.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="109">
   <si>
     <t>N2</t>
   </si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>10.1063/1.2222065</t>
-  </si>
-  <si>
-    <t>p-xylene</t>
   </si>
 </sst>
 </file>
@@ -1577,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2139730168"/>
-        <c:axId val="2139735752"/>
+        <c:axId val="2070716696"/>
+        <c:axId val="2070460552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2139730168"/>
+        <c:axId val="2070716696"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1618,12 +1615,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139735752"/>
+        <c:crossAx val="2070460552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139735752"/>
+        <c:axId val="2070460552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1653,7 +1650,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139730168"/>
+        <c:crossAx val="2070716696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2334,11 +2331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064502696"/>
-        <c:axId val="2064505688"/>
+        <c:axId val="2070503320"/>
+        <c:axId val="2070506312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064502696"/>
+        <c:axId val="2070503320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2348,12 +2345,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064505688"/>
+        <c:crossAx val="2070506312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064505688"/>
+        <c:axId val="2070506312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2388,7 +2385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064502696"/>
+        <c:crossAx val="2070503320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3106,11 +3103,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064542296"/>
-        <c:axId val="2064545288"/>
+        <c:axId val="2070784408"/>
+        <c:axId val="2070787400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064542296"/>
+        <c:axId val="2070784408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3120,12 +3117,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064545288"/>
+        <c:crossAx val="2070787400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064545288"/>
+        <c:axId val="2070787400"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3150,7 +3147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064542296"/>
+        <c:crossAx val="2070784408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3273,11 +3270,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064568040"/>
-        <c:axId val="2064571128"/>
+        <c:axId val="2070810120"/>
+        <c:axId val="2070813208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064568040"/>
+        <c:axId val="2070810120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3287,12 +3284,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064571128"/>
+        <c:crossAx val="2070813208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064571128"/>
+        <c:axId val="2070813208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3303,7 +3300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064568040"/>
+        <c:crossAx val="2070810120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3411,11 +3408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064595240"/>
-        <c:axId val="2064598264"/>
+        <c:axId val="2070837032"/>
+        <c:axId val="2070840056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064595240"/>
+        <c:axId val="2070837032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3425,12 +3422,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064598264"/>
+        <c:crossAx val="2070840056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064598264"/>
+        <c:axId val="2070840056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064595240"/>
+        <c:crossAx val="2070837032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3555,11 +3552,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064622440"/>
-        <c:axId val="2064625400"/>
+        <c:axId val="2070863992"/>
+        <c:axId val="2070866952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064622440"/>
+        <c:axId val="2070863992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3569,12 +3566,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064625400"/>
+        <c:crossAx val="2070866952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064625400"/>
+        <c:axId val="2070866952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,7 +3582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064622440"/>
+        <c:crossAx val="2070863992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4085,10 +4082,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BW134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4080" activePane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <pane xSplit="4080" topLeftCell="F1" activePane="topRight"/>
       <selection activeCell="B3" sqref="B3:B30"/>
-      <selection pane="topRight" activeCell="W105" sqref="W105"/>
+      <selection pane="topRight" activeCell="U73" sqref="U73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5813,7 +5810,7 @@
         <v>57</v>
       </c>
       <c r="BU9" s="5" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="BV9" s="5" t="s">
         <v>13</v>
@@ -9442,7 +9439,7 @@
         <v>57</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>13</v>
@@ -9486,7 +9483,7 @@
         <v>334</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" ref="H44:L44" si="10">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="H44:I44" si="10">IF(ISBLANK(H42),LOOKUP(H41,$A$100:$A$108,$F$100:$F$108),H43*LOOKUP(H41,$A$100:$A$108,$F$100:$F$108)+(1-H43)*LOOKUP(H42,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="I44" s="5">
@@ -9515,7 +9512,7 @@
         <v>13.174999999999979</v>
       </c>
       <c r="D45" s="14">
-        <f t="shared" ref="D45:L45" si="12">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D45:H45" si="12">IF(ISBLANK(D42), 4*(LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D43*LOOKUP(D41,$A$101:$A$108,$B$101:$B$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$C$101:$C$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D43*LOOKUP(D41,$A$101:$A$108,$D$101:$D$108)+(1-D43)*LOOKUP(D42,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>13.174999999999979</v>
       </c>
       <c r="E45" s="14">
@@ -10438,7 +10435,7 @@
         <v>57</v>
       </c>
       <c r="U72" s="5" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>13</v>
@@ -10558,7 +10555,7 @@
         <v>334</v>
       </c>
       <c r="R75" s="5">
-        <f t="shared" ref="R75:W75" si="26">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
+        <f t="shared" ref="R75:S75" si="26">IF(ISBLANK(R73),LOOKUP(R72,$A$100:$A$108,$F$100:$F$108),R74*LOOKUP(R72,$A$100:$A$108,$F$100:$F$108)+(1-R74)*LOOKUP(R73,$A$100:$A$108,$F$100:$F$108))</f>
         <v>334</v>
       </c>
       <c r="S75" s="5">
@@ -10591,7 +10588,7 @@
         <v>17.073470400000005</v>
       </c>
       <c r="D76" s="14">
-        <f t="shared" ref="D76:W76" si="28">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
+        <f t="shared" ref="D76:S76" si="28">IF(ISBLANK(D73), 4*(LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)-$B$100)^2+(LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)-$C$100)^2+(LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)-$D$100)^2,4*((D74*LOOKUP(D72,$A$101:$A$108,$B$101:$B$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$B$101:$B$108))-$B$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$C$101:$C$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$C$101:$C$108))-$C$100)^2+((D74*LOOKUP(D72,$A$101:$A$108,$D$101:$D$108)+(1-D74)*LOOKUP(D73,$A$101:$A$108,$D$101:$D$108))-$D$100)^2)</f>
         <v>17.073470400000005</v>
       </c>
       <c r="E76" s="14">

</xml_diff>